<commit_message>
CT update keywords and data
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/customer_tagging_test_data.xlsx
+++ b/TestData/Web_POS/Billing/customer_tagging_test_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="117">
   <si>
     <t xml:space="preserve">TC_Id</t>
   </si>
@@ -76,10 +76,13 @@
     <t xml:space="preserve">group</t>
   </si>
   <si>
-    <t xml:space="preserve">tax_invoice </t>
+    <t xml:space="preserve">tax_invoice</t>
   </si>
   <si>
     <t xml:space="preserve">legal_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uin_number</t>
   </si>
   <si>
     <t xml:space="preserve">gst_number</t>
@@ -258,18 +261,12 @@
     <t xml:space="preserve">QBSB-Specificqty-Flat-rupees</t>
   </si>
   <si>
-    <t xml:space="preserve">8906118410781 : 2, 8906118412556 : 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC_10</t>
   </si>
   <si>
     <t xml:space="preserve">QBSB-Anyqty-Flat-percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">8906118410781 : 1, 8906118412556 : 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC_11</t>
   </si>
   <si>
@@ -285,6 +282,12 @@
     <t xml:space="preserve">QBSB-Any____qty-Buypool-Flat-Rupees</t>
   </si>
   <si>
+    <t xml:space="preserve">GST1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29GGGGG1314R9Z6</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_13</t>
   </si>
   <si>
@@ -294,19 +297,25 @@
     <t xml:space="preserve">8906118410781 : 5</t>
   </si>
   <si>
+    <t xml:space="preserve">UIN1</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_14</t>
   </si>
   <si>
     <t xml:space="preserve">QBSB-Any Qty-Buy pool-Fixed-all</t>
   </si>
   <si>
+    <t xml:space="preserve">Existing GST</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_15</t>
   </si>
   <si>
     <t xml:space="preserve">QBSB-Any Qty-get pool-spf-Rupees</t>
   </si>
   <si>
-    <t xml:space="preserve">8906118412761 : 1</t>
+    <t xml:space="preserve">GST2</t>
   </si>
   <si>
     <t xml:space="preserve">TC_16</t>
@@ -315,37 +324,49 @@
     <t xml:space="preserve">QBSB-Any Qty-get pool-spf-Fixed-each</t>
   </si>
   <si>
-    <t xml:space="preserve">8906118412761 : 1, 8906118412556 : 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC_17</t>
   </si>
   <si>
     <t xml:space="preserve">QBSB-Any Get pool-spf-Fixed-all</t>
   </si>
   <si>
-    <t xml:space="preserve">8906118412556 : 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC_18</t>
   </si>
   <si>
     <t xml:space="preserve">QBSB-Specificity-Flat-fixed-all</t>
   </si>
   <si>
+    <t xml:space="preserve">Delete GST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delgst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QBSB-Specificity-Flat-fixed-each</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete UIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deluin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-perc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Null</t>
   </si>
   <si>
-    <t xml:space="preserve">TC_19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Specificity-Flat-fixed-each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-perc</t>
+    <t xml:space="preserve">goagst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30AAAAP0267H1Z1 </t>
   </si>
   <si>
     <t xml:space="preserve">TC_21</t>
@@ -354,15 +375,15 @@
     <t xml:space="preserve">QBSB-Any____Qty-get pool-any-rupees</t>
   </si>
   <si>
+    <t xml:space="preserve">UIN3</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_22</t>
   </si>
   <si>
     <t xml:space="preserve">QBSB-Any____Qty-get pool-any-fixed-each</t>
   </si>
   <si>
-    <t xml:space="preserve">8906118412761 : 1, 8906118412556 : 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC_23</t>
   </si>
   <si>
@@ -379,9 +400,6 @@
   </si>
   <si>
     <t xml:space="preserve">QBSB-Any qty-flat-rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GST2</t>
   </si>
   <si>
     <t xml:space="preserve">TC_26</t>
@@ -425,7 +443,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-409]M/D/YYYY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -486,6 +504,22 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -555,7 +589,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -597,6 +631,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -679,13 +721,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X100"/>
+  <dimension ref="A1:Y63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V10" activeCellId="0" sqref="V10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V13" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W28" activeCellId="0" sqref="W28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -701,9 +743,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="1" width="29.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="23.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="28.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="28.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -776,25 +818,28 @@
       <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F2" s="7" t="n">
         <v>123456</v>
@@ -806,10 +851,10 @@
         <v>500</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>1</v>
@@ -818,40 +863,40 @@
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O2" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F3" s="7" t="n">
         <v>123456</v>
@@ -863,10 +908,10 @@
         <v>500</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>1</v>
@@ -875,40 +920,40 @@
         <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O3" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F4" s="7" t="n">
         <v>123456</v>
@@ -920,10 +965,10 @@
         <v>300</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>1</v>
@@ -932,40 +977,40 @@
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O4" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F5" s="7" t="n">
         <v>123456</v>
@@ -977,10 +1022,10 @@
         <v>400</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>1</v>
@@ -989,43 +1034,43 @@
         <v>2</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O5" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S5" s="3"/>
-      <c r="X5" s="0" t="n">
+      <c r="Y5" s="0" t="n">
         <v>431103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6" s="7" t="n">
         <v>123456</v>
@@ -1037,10 +1082,10 @@
         <v>800</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>1</v>
@@ -1049,40 +1094,40 @@
         <v>2</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O6" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" s="7" t="n">
         <v>123456</v>
@@ -1094,10 +1139,10 @@
         <v>600</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K7" s="1" t="n">
         <v>1</v>
@@ -1106,40 +1151,40 @@
         <v>2</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O7" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" s="7" t="n">
         <v>123456</v>
@@ -1151,10 +1196,10 @@
         <v>600</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K8" s="1" t="n">
         <v>1</v>
@@ -1163,40 +1208,40 @@
         <v>2</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O8" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" s="7" t="n">
         <v>123456</v>
@@ -1208,10 +1253,10 @@
         <v>600</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K9" s="1" t="n">
         <v>1</v>
@@ -1220,40 +1265,40 @@
         <v>2</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O9" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F10" s="7" t="n">
         <v>123456</v>
@@ -1265,10 +1310,10 @@
         <v>600</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K10" s="1" t="n">
         <v>1</v>
@@ -1277,43 +1322,43 @@
         <v>2</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O10" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S10" s="3"/>
-      <c r="V10" s="0" t="n">
+      <c r="W10" s="0" t="n">
         <v>9876543212</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="7" t="n">
         <v>123456</v>
@@ -1325,7 +1370,7 @@
         <v>600</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>60</v>
@@ -1337,40 +1382,40 @@
         <v>2</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O11" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F12" s="7" t="n">
         <v>123456</v>
@@ -1382,52 +1427,52 @@
         <v>600</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="N12" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O12" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F13" s="7" t="n">
         <v>123456</v>
@@ -1439,10 +1484,10 @@
         <v>600</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
@@ -1451,40 +1496,49 @@
         <v>1</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O13" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P13" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+      <c r="S13" s="11"/>
+      <c r="T13" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="V13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y13" s="0" t="n">
+        <v>431103</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F14" s="7" t="n">
         <v>123456</v>
@@ -1496,10 +1550,10 @@
         <v>600</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>1</v>
@@ -1508,40 +1562,49 @@
         <v>1</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O14" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S14" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="S14" s="11"/>
+      <c r="T14" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="U14" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <v>431103</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F15" s="7" t="n">
         <v>123456</v>
@@ -1553,10 +1616,10 @@
         <v>600</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>1</v>
@@ -1565,40 +1628,51 @@
         <v>1</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O15" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S15" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="S15" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="T15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>9876543212</v>
+      </c>
+      <c r="Y15" s="0" t="n">
+        <v>431103</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F16" s="7" t="n">
         <v>123456</v>
@@ -1610,10 +1684,10 @@
         <v>600</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="K16" s="1" t="n">
         <v>1</v>
@@ -1622,40 +1696,49 @@
         <v>1</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="O16" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P16" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T16" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <v>9876543212</v>
+      </c>
+      <c r="Y16" s="0" t="n">
+        <v>431103</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F17" s="7" t="n">
         <v>123456</v>
@@ -1667,10 +1750,10 @@
         <v>600</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K17" s="1" t="n">
         <v>1</v>
@@ -1679,40 +1762,49 @@
         <v>1</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="O17" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S17" s="3"/>
+      <c r="T17" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <v>9876543212</v>
+      </c>
+      <c r="X17" s="0" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F18" s="7" t="n">
         <v>123456</v>
@@ -1724,10 +1816,10 @@
         <v>600</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="K18" s="1" t="n">
         <v>1</v>
@@ -1736,40 +1828,49 @@
         <v>3</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="O18" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P18" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S18" s="3"/>
-    </row>
-    <row r="19" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>9876543212</v>
+      </c>
+      <c r="X18" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F19" s="7" t="n">
         <v>123456</v>
@@ -1781,10 +1882,10 @@
         <v>600</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K19" s="1" t="n">
         <v>1</v>
@@ -1793,42 +1894,54 @@
         <v>1</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O19" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P19" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S19" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+      <c r="S19" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="T19" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="U19" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="V19" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="W19" s="0" t="n">
+        <v>8149214985</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F20" s="7" t="n">
         <v>123456</v>
@@ -1840,10 +1953,10 @@
         <v>600</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K20" s="1" t="n">
         <v>1</v>
@@ -1852,42 +1965,57 @@
         <v>1</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O20" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P20" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S20" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+      <c r="S20" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="T20" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="U20" s="12" t="n">
+        <v>123456789876543</v>
+      </c>
+      <c r="V20" s="12" t="n">
+        <v>123456789876543</v>
+      </c>
+      <c r="W20" s="0" t="n">
+        <v>8149214985</v>
+      </c>
+      <c r="Y20" s="0" t="n">
+        <v>431103</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F21" s="7" t="n">
         <v>123456</v>
@@ -1899,10 +2027,10 @@
         <v>600</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="K21" s="1" t="n">
         <v>1</v>
@@ -1911,42 +2039,52 @@
         <v>1</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="O21" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+      <c r="T21" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y21" s="0" t="n">
+        <v>431103</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D22" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F22" s="7" t="n">
         <v>123456</v>
@@ -1958,10 +2096,10 @@
         <v>600</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="K22" s="1" t="n">
         <v>1</v>
@@ -1970,42 +2108,51 @@
         <v>3</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="O22" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P22" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+      <c r="T22" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="U22" s="0" t="n">
+        <v>123456765445434</v>
+      </c>
+      <c r="Y22" s="0" t="n">
+        <v>431103</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D23" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F23" s="7" t="n">
         <v>123456</v>
@@ -2017,10 +2164,10 @@
         <v>600</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="K23" s="1" t="n">
         <v>1</v>
@@ -2029,42 +2176,45 @@
         <v>3</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="O23" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P23" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+      <c r="Y23" s="0" t="n">
+        <v>431103</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D24" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F24" s="7" t="n">
         <v>123456</v>
@@ -2076,51 +2226,51 @@
         <v>600</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="L24" s="1" t="n">
         <v>2</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="O24" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P24" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D25" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F25" s="7" t="n">
         <v>123456</v>
@@ -2132,10 +2282,10 @@
         <v>600</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K25" s="1" t="n">
         <v>1</v>
@@ -2144,42 +2294,51 @@
         <v>2</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="O25" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P25" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+      <c r="T25" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W25" s="0" t="n">
+        <v>8149214985</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F26" s="7" t="n">
         <v>123456</v>
@@ -2191,10 +2350,10 @@
         <v>600</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="K26" s="1" t="n">
         <v>1</v>
@@ -2202,49 +2361,55 @@
       <c r="L26" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="M26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N26" s="0" t="s">
+      <c r="M26" s="0" t="s">
         <v>31</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="O26" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="V26" s="0" t="n">
-        <v>9876543212</v>
-      </c>
-      <c r="W26" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+      <c r="T26" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="U26" s="0" t="n">
+        <v>123456765445434</v>
+      </c>
+      <c r="W26" s="0" t="n">
+        <v>8149214985</v>
+      </c>
+      <c r="X26" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D27" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F27" s="7" t="n">
         <v>123456</v>
@@ -2256,10 +2421,10 @@
         <v>600</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="K27" s="1" t="n">
         <v>1</v>
@@ -2267,49 +2432,49 @@
       <c r="L27" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N27" s="0" t="s">
+      <c r="M27" s="0" t="s">
         <v>31</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="O27" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P27" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="T27" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="U27" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>108</v>
+      </c>
+      <c r="V27" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D28" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F28" s="7" t="n">
         <v>123456</v>
@@ -2321,10 +2486,10 @@
         <v>600</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="K28" s="1" t="n">
         <v>1</v>
@@ -2332,43 +2497,46 @@
       <c r="L28" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N28" s="0" t="s">
+      <c r="M28" s="0" t="s">
         <v>31</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="O28" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>83</v>
+        <v>92</v>
+      </c>
+      <c r="W28" s="0" t="n">
+        <v>656765</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D29" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F29" s="7" t="n">
         <v>123456</v>
@@ -2380,10 +2548,10 @@
         <v>600</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="K29" s="1" t="n">
         <v>1</v>
@@ -2392,42 +2560,42 @@
         <v>1</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O29" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P29" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q29" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D30" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F30" s="7" t="n">
         <v>123456</v>
@@ -2439,10 +2607,10 @@
         <v>600</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="K30" s="1" t="n">
         <v>1</v>
@@ -2451,22 +2619,22 @@
         <v>1</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O30" s="9" t="n">
         <v>45386</v>
       </c>
       <c r="P30" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q30" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S30" s="3"/>
     </row>
@@ -2873,43 +3041,6 @@
       <c r="Q63" s="9"/>
       <c r="S63" s="3"/>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
second test data update
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/customer_tagging_test_data.xlsx
+++ b/TestData/Web_POS/Billing/customer_tagging_test_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="116">
   <si>
     <t xml:space="preserve">TC_Id</t>
   </si>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">TC_01</t>
   </si>
   <si>
-    <t xml:space="preserve">307260624P3E </t>
+    <t xml:space="preserve">307260624P3E</t>
   </si>
   <si>
     <t xml:space="preserve">zwshashank.agrawal@teampureplay.com</t>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">TC_02</t>
   </si>
   <si>
-    <t xml:space="preserve">30726062464i </t>
+    <t xml:space="preserve">30726062464i</t>
   </si>
   <si>
     <t xml:space="preserve">userone_p8 </t>
@@ -184,6 +184,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -193,6 +194,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8906118412556 : 3</t>
     </r>
@@ -207,52 +209,13 @@
     <t xml:space="preserve">QBSB-any____qty-Getpool-Anyqty-Free</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8906118410781 : 2, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">8906118412556 : 2</t>
-    </r>
+    <t xml:space="preserve">8906118410781 : 2, 8906118412556 : 2</t>
   </si>
   <si>
     <t xml:space="preserve">TC_08</t>
   </si>
   <si>
     <t xml:space="preserve">QBSB-Specificqty-Flat-percentage</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8906118410781 : 2,  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">8906118412556 : 3</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">TC_09</t>
@@ -443,7 +406,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-409]M/D/YYYY"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -493,17 +456,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <i val="true"/>
@@ -589,7 +541,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -630,15 +582,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -723,8 +671,8 @@
   </sheetPr>
   <dimension ref="A1:Y63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V13" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W28" activeCellId="0" sqref="W28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1153,7 +1101,7 @@
       <c r="M7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="N7" s="1" t="s">
         <v>50</v>
       </c>
       <c r="O7" s="9" t="n">
@@ -1210,7 +1158,7 @@
       <c r="M8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="N8" s="1" t="s">
         <v>50</v>
       </c>
       <c r="O8" s="9" t="n">
@@ -1265,7 +1213,7 @@
         <v>2</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>32</v>
@@ -1286,7 +1234,7 @@
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>26</v>
@@ -1313,7 +1261,7 @@
         <v>29</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K10" s="1" t="n">
         <v>1</v>
@@ -1344,9 +1292,9 @@
         <v>9876543212</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>26</v>
@@ -1373,7 +1321,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K11" s="1" t="n">
         <v>1</v>
@@ -1401,9 +1349,9 @@
       </c>
       <c r="S11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
@@ -1430,16 +1378,16 @@
         <v>29</v>
       </c>
       <c r="J12" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="K12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>32</v>
@@ -1458,9 +1406,9 @@
       </c>
       <c r="S12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>26</v>
@@ -1487,7 +1435,7 @@
         <v>29</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
@@ -1496,7 +1444,7 @@
         <v>1</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>32</v>
@@ -1513,20 +1461,20 @@
       <c r="R13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S13" s="11"/>
+      <c r="S13" s="10"/>
       <c r="T13" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="V13" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="V13" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="Y13" s="0" t="n">
         <v>431103</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>26</v>
@@ -1553,16 +1501,16 @@
         <v>29</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="K14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>32</v>
@@ -1579,12 +1527,12 @@
       <c r="R14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S14" s="11"/>
+      <c r="S14" s="10"/>
       <c r="T14" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="U14" s="12" t="s">
-        <v>67</v>
+        <v>70</v>
+      </c>
+      <c r="U14" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="Y14" s="0" t="n">
         <v>431103</v>
@@ -1592,7 +1540,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>26</v>
@@ -1619,7 +1567,7 @@
         <v>29</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>1</v>
@@ -1628,7 +1576,7 @@
         <v>1</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>32</v>
@@ -1645,11 +1593,11 @@
       <c r="R15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S15" s="11" t="s">
-        <v>74</v>
+      <c r="S15" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="T15" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W15" s="0" t="n">
         <v>9876543212</v>
@@ -1660,7 +1608,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>26</v>
@@ -1687,7 +1635,7 @@
         <v>29</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K16" s="1" t="n">
         <v>1</v>
@@ -1715,7 +1663,7 @@
       </c>
       <c r="S16" s="3"/>
       <c r="T16" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W16" s="0" t="n">
         <v>9876543212</v>
@@ -1726,7 +1674,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>26</v>
@@ -1753,7 +1701,7 @@
         <v>29</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K17" s="1" t="n">
         <v>1</v>
@@ -1781,18 +1729,18 @@
       </c>
       <c r="S17" s="3"/>
       <c r="T17" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W17" s="0" t="n">
         <v>9876543212</v>
       </c>
       <c r="X17" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>26</v>
@@ -1819,7 +1767,7 @@
         <v>29</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K18" s="1" t="n">
         <v>1</v>
@@ -1847,18 +1795,18 @@
       </c>
       <c r="S18" s="3"/>
       <c r="T18" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W18" s="0" t="n">
         <v>9876543212</v>
       </c>
       <c r="X18" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>26</v>
@@ -1885,7 +1833,7 @@
         <v>29</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K19" s="1" t="n">
         <v>1</v>
@@ -1911,17 +1859,17 @@
       <c r="R19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S19" s="11" t="s">
+      <c r="S19" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="T19" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="T19" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="U19" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="V19" s="12" t="s">
-        <v>67</v>
+      <c r="U19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="V19" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="W19" s="0" t="n">
         <v>8149214985</v>
@@ -1929,7 +1877,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>26</v>
@@ -1956,7 +1904,7 @@
         <v>29</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K20" s="1" t="n">
         <v>1</v>
@@ -1982,16 +1930,16 @@
       <c r="R20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S20" s="11" t="s">
+      <c r="S20" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="T20" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="T20" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="U20" s="12" t="n">
+      <c r="U20" s="11" t="n">
         <v>123456789876543</v>
       </c>
-      <c r="V20" s="12" t="n">
+      <c r="V20" s="11" t="n">
         <v>123456789876543</v>
       </c>
       <c r="W20" s="0" t="n">
@@ -2003,7 +1951,7 @@
     </row>
     <row r="21" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>26</v>
@@ -2030,7 +1978,7 @@
         <v>29</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K21" s="1" t="n">
         <v>1</v>
@@ -2057,14 +2005,14 @@
         <v>35</v>
       </c>
       <c r="S21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="T21" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="T21" s="0" t="s">
-        <v>93</v>
       </c>
       <c r="U21" s="1"/>
       <c r="V21" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Y21" s="0" t="n">
         <v>431103</v>
@@ -2072,7 +2020,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>26</v>
@@ -2099,7 +2047,7 @@
         <v>29</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K22" s="1" t="n">
         <v>1</v>
@@ -2126,10 +2074,10 @@
         <v>35</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T22" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U22" s="0" t="n">
         <v>123456765445434</v>
@@ -2140,7 +2088,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>26</v>
@@ -2167,7 +2115,7 @@
         <v>29</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K23" s="1" t="n">
         <v>1</v>
@@ -2194,7 +2142,7 @@
         <v>35</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y23" s="0" t="n">
         <v>431103</v>
@@ -2202,7 +2150,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>26</v>
@@ -2229,7 +2177,7 @@
         <v>29</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L24" s="1" t="n">
         <v>2</v>
@@ -2253,12 +2201,12 @@
         <v>35</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>26</v>
@@ -2285,7 +2233,7 @@
         <v>29</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K25" s="1" t="n">
         <v>1</v>
@@ -2312,13 +2260,13 @@
         <v>35</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T25" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W25" s="0" t="n">
         <v>8149214985</v>
@@ -2326,7 +2274,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>26</v>
@@ -2353,7 +2301,7 @@
         <v>29</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K26" s="1" t="n">
         <v>1</v>
@@ -2380,10 +2328,10 @@
         <v>35</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T26" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U26" s="0" t="n">
         <v>123456765445434</v>
@@ -2392,12 +2340,12 @@
         <v>8149214985</v>
       </c>
       <c r="X26" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>26</v>
@@ -2424,7 +2372,7 @@
         <v>29</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K27" s="1" t="n">
         <v>1</v>
@@ -2451,18 +2399,18 @@
         <v>35</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T27" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="V27" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="V27" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>26</v>
@@ -2489,7 +2437,7 @@
         <v>29</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K28" s="1" t="n">
         <v>1</v>
@@ -2516,7 +2464,7 @@
         <v>35</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W28" s="0" t="n">
         <v>656765</v>
@@ -2524,7 +2472,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
@@ -2551,7 +2499,7 @@
         <v>29</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K29" s="1" t="n">
         <v>1</v>
@@ -2560,7 +2508,7 @@
         <v>1</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>32</v>
@@ -2578,12 +2526,12 @@
         <v>35</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>26</v>
@@ -2610,16 +2558,16 @@
         <v>29</v>
       </c>
       <c r="J30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M30" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="K30" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L30" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Suit Execution 23 passed
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/customer_tagging_test_data.xlsx
+++ b/TestData/Web_POS/Billing/customer_tagging_test_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="123">
   <si>
     <t xml:space="preserve">TC_Id</t>
   </si>
@@ -100,6 +100,9 @@
     <t xml:space="preserve">salesperson_name</t>
   </si>
   <si>
+    <t xml:space="preserve">new_city</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_01</t>
   </si>
   <si>
@@ -148,7 +151,7 @@
     <t xml:space="preserve">TC_03</t>
   </si>
   <si>
-    <t xml:space="preserve">307260624Wa9 </t>
+    <t xml:space="preserve">307260624Wa9</t>
   </si>
   <si>
     <t xml:space="preserve">QBSB-any___qty-Flat-Fixed-Each</t>
@@ -157,7 +160,7 @@
     <t xml:space="preserve">TC_04</t>
   </si>
   <si>
-    <t xml:space="preserve">3070907243ZY </t>
+    <t xml:space="preserve">3070907243ZY</t>
   </si>
   <si>
     <t xml:space="preserve">userone_p9</t>
@@ -304,37 +307,43 @@
     <t xml:space="preserve">Null</t>
   </si>
   <si>
-    <t xml:space="preserve">goagst</t>
+    <t xml:space="preserve">arunachalgst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12AAACB1534F1ZH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasighat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-rupees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UIN3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-fixed-each</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-fixed-all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QBSB-Any____Qty-get pool-spf-perc</t>
   </si>
   <si>
     <t xml:space="preserve">30AAAAP0267H1Z1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UIN3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-fixed-each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-fixed-all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-spf-perc</t>
   </si>
   <si>
     <t xml:space="preserve">TC_25</t>
@@ -525,7 +534,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -548,6 +557,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -653,10 +666,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z63"/>
+  <dimension ref="A1:AA63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="1" sqref="E4 E3"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -759,24 +772,27 @@
       <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="7" t="n">
+      <c r="E2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G2" s="1" t="n">
@@ -786,11 +802,11 @@
         <v>500</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="8" t="s">
         <v>31</v>
       </c>
+      <c r="J2" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="K2" s="1" t="n">
         <v>1</v>
       </c>
@@ -798,42 +814,42 @@
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O2" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="9" t="s">
+      <c r="P2" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q2" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F3" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G3" s="0" t="n">
@@ -843,10 +859,10 @@
         <v>500</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>40</v>
+        <v>31</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>1</v>
@@ -855,42 +871,42 @@
         <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O3" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="9" t="s">
+      <c r="P3" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q3" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F4" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G4" s="0" t="n">
@@ -900,10 +916,10 @@
         <v>300</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>43</v>
+        <v>31</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>1</v>
@@ -912,42 +928,42 @@
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O4" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O4" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q4" s="9" t="s">
+      <c r="P4" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q4" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="7" t="n">
+      <c r="E5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G5" s="0" t="n">
@@ -957,10 +973,10 @@
         <v>400</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>47</v>
+        <v>31</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>1</v>
@@ -969,48 +985,48 @@
         <v>2</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O5" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" s="9" t="s">
+      <c r="P5" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q5" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S5" s="3"/>
       <c r="Y5" s="0" t="n">
         <v>411001</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="7" t="n">
+      <c r="E6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G6" s="0" t="n">
@@ -1020,10 +1036,10 @@
         <v>800</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>51</v>
+        <v>31</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>1</v>
@@ -1032,42 +1048,42 @@
         <v>2</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O6" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" s="9" t="s">
+      <c r="P6" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q6" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="7" t="n">
+      <c r="E7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G7" s="0" t="n">
@@ -1077,10 +1093,10 @@
         <v>600</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>53</v>
+        <v>31</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="K7" s="1" t="n">
         <v>1</v>
@@ -1089,42 +1105,42 @@
         <v>2</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O7" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O7" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q7" s="9" t="s">
+      <c r="P7" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q7" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="7" t="n">
+      <c r="E8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -1134,10 +1150,10 @@
         <v>600</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>55</v>
+        <v>31</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="K8" s="1" t="n">
         <v>1</v>
@@ -1146,42 +1162,42 @@
         <v>2</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O8" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O8" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P8" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q8" s="9" t="s">
+      <c r="P8" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q8" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="7" t="n">
+      <c r="E9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G9" s="0" t="n">
@@ -1191,10 +1207,10 @@
         <v>600</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>57</v>
+        <v>31</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="K9" s="1" t="n">
         <v>1</v>
@@ -1203,42 +1219,42 @@
         <v>2</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O9" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O9" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P9" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q9" s="9" t="s">
+      <c r="P9" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q9" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="7" t="n">
+      <c r="E10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G10" s="0" t="n">
@@ -1248,10 +1264,10 @@
         <v>600</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>59</v>
+        <v>31</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="K10" s="1" t="n">
         <v>1</v>
@@ -1260,22 +1276,22 @@
         <v>2</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O10" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O10" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P10" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q10" s="9" t="s">
+      <c r="P10" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q10" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S10" s="3"/>
       <c r="W10" s="0" t="n">
@@ -1284,21 +1300,21 @@
     </row>
     <row r="11" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="7" t="n">
+      <c r="E11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G11" s="0" t="n">
@@ -1308,10 +1324,10 @@
         <v>600</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>61</v>
+        <v>31</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="K11" s="1" t="n">
         <v>1</v>
@@ -1320,42 +1336,42 @@
         <v>2</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O11" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O11" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q11" s="9" t="s">
+      <c r="P11" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q11" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="7" t="n">
+      <c r="E12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G12" s="0" t="n">
@@ -1365,10 +1381,10 @@
         <v>600</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>63</v>
+        <v>31</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="K12" s="1" t="n">
         <v>1</v>
@@ -1377,42 +1393,42 @@
         <v>1</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O12" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O12" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q12" s="9" t="s">
+      <c r="P12" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q12" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="7" t="n">
+      <c r="E13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G13" s="0" t="n">
@@ -1422,10 +1438,10 @@
         <v>600</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
@@ -1434,29 +1450,29 @@
         <v>1</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O13" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O13" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q13" s="9" t="s">
+      <c r="P13" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q13" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S13" s="10"/>
+        <v>37</v>
+      </c>
+      <c r="S13" s="11"/>
       <c r="T13" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="V13" s="11" t="s">
         <v>68</v>
+      </c>
+      <c r="V13" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="Y13" s="0" t="n">
         <v>411001</v>
@@ -1464,21 +1480,21 @@
     </row>
     <row r="14" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="7" t="n">
+      <c r="E14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G14" s="0" t="n">
@@ -1488,10 +1504,10 @@
         <v>600</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>1</v>
@@ -1500,29 +1516,29 @@
         <v>1</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O14" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O14" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P14" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q14" s="9" t="s">
+      <c r="P14" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q14" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S14" s="10"/>
+        <v>37</v>
+      </c>
+      <c r="S14" s="11"/>
       <c r="T14" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="U14" s="11" t="s">
-        <v>68</v>
+        <v>73</v>
+      </c>
+      <c r="U14" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="Y14" s="0" t="n">
         <v>411001</v>
@@ -1530,21 +1546,21 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="7" t="n">
+      <c r="E15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G15" s="0" t="n">
@@ -1554,10 +1570,10 @@
         <v>600</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>1</v>
@@ -1566,28 +1582,28 @@
         <v>1</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O15" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O15" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q15" s="9" t="s">
+      <c r="P15" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q15" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S15" s="10" t="s">
-        <v>75</v>
+        <v>37</v>
+      </c>
+      <c r="S15" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="T15" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="W15" s="0" t="n">
         <v>9876543212</v>
@@ -1598,21 +1614,21 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="7" t="n">
+      <c r="E16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G16" s="0" t="n">
@@ -1622,10 +1638,10 @@
         <v>600</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K16" s="1" t="n">
         <v>1</v>
@@ -1634,26 +1650,26 @@
         <v>1</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O16" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O16" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q16" s="9" t="s">
+      <c r="P16" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q16" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R16" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S16" s="3"/>
       <c r="T16" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="W16" s="0" t="n">
         <v>9876543212</v>
@@ -1664,21 +1680,21 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="7" t="n">
+      <c r="E17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G17" s="0" t="n">
@@ -1688,10 +1704,10 @@
         <v>600</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K17" s="1" t="n">
         <v>1</v>
@@ -1700,51 +1716,51 @@
         <v>1</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O17" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O17" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P17" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q17" s="9" t="s">
+      <c r="P17" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q17" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S17" s="3"/>
       <c r="T17" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="W17" s="0" t="n">
         <v>9876543212</v>
       </c>
       <c r="X17" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="7" t="n">
+      <c r="E18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G18" s="0" t="n">
@@ -1754,10 +1770,10 @@
         <v>600</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K18" s="1" t="n">
         <v>1</v>
@@ -1766,51 +1782,51 @@
         <v>3</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O18" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O18" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q18" s="9" t="s">
+      <c r="P18" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q18" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R18" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S18" s="3"/>
       <c r="T18" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="W18" s="0" t="n">
         <v>9876543212</v>
       </c>
       <c r="X18" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="7" t="n">
+      <c r="E19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G19" s="0" t="n">
@@ -1820,10 +1836,10 @@
         <v>600</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K19" s="1" t="n">
         <v>1</v>
@@ -1832,34 +1848,34 @@
         <v>1</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O19" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O19" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P19" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q19" s="9" t="s">
+      <c r="P19" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q19" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S19" s="10" t="s">
-        <v>85</v>
+        <v>37</v>
+      </c>
+      <c r="S19" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="T19" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="U19" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="V19" s="11" t="s">
-        <v>68</v>
+        <v>87</v>
+      </c>
+      <c r="U19" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="V19" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="W19" s="0" t="n">
         <v>8149214985</v>
@@ -1870,21 +1886,21 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="7" t="n">
+      <c r="E20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G20" s="0" t="n">
@@ -1894,10 +1910,10 @@
         <v>600</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K20" s="1" t="n">
         <v>1</v>
@@ -1906,33 +1922,33 @@
         <v>1</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O20" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O20" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P20" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q20" s="9" t="s">
+      <c r="P20" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q20" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S20" s="10" t="s">
-        <v>89</v>
+        <v>37</v>
+      </c>
+      <c r="S20" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="T20" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="U20" s="11" t="n">
+        <v>91</v>
+      </c>
+      <c r="U20" s="12" t="n">
         <v>123456789876543</v>
       </c>
-      <c r="V20" s="11" t="n">
+      <c r="V20" s="12" t="n">
         <v>123456789876543</v>
       </c>
       <c r="W20" s="0" t="n">
@@ -1942,23 +1958,23 @@
         <v>411001</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D21" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="7" t="n">
+      <c r="E21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G21" s="0" t="n">
@@ -1968,10 +1984,10 @@
         <v>600</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K21" s="1" t="n">
         <v>1</v>
@@ -1980,54 +1996,57 @@
         <v>1</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O21" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O21" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P21" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q21" s="9" t="s">
+      <c r="P21" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q21" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R21" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="T21" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="U21" s="1"/>
-      <c r="V21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y21" s="0" t="n">
-        <v>411001</v>
+      <c r="V21" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y21" s="12" t="n">
+        <v>791102</v>
+      </c>
+      <c r="AA21" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D22" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="7" t="n">
+      <c r="E22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G22" s="0" t="n">
@@ -2037,10 +2056,10 @@
         <v>600</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K22" s="1" t="n">
         <v>1</v>
@@ -2049,28 +2068,28 @@
         <v>3</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O22" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O22" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P22" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q22" s="9" t="s">
+      <c r="P22" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q22" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="T22" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="U22" s="0" t="n">
         <v>123456765445434</v>
@@ -2081,21 +2100,21 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D23" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="7" t="n">
+      <c r="E23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G23" s="0" t="n">
@@ -2105,10 +2124,10 @@
         <v>600</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K23" s="1" t="n">
         <v>1</v>
@@ -2117,25 +2136,25 @@
         <v>3</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O23" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O23" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P23" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q23" s="9" t="s">
+      <c r="P23" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q23" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R23" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Y23" s="0" t="n">
         <v>411001</v>
@@ -2143,21 +2162,21 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D24" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="7" t="n">
+      <c r="E24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G24" s="0" t="n">
@@ -2167,34 +2186,34 @@
         <v>600</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="L24" s="1" t="n">
         <v>2</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O24" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O24" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P24" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q24" s="9" t="s">
+      <c r="P24" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q24" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R24" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Y24" s="0" t="n">
         <v>411001</v>
@@ -2202,21 +2221,21 @@
     </row>
     <row r="25" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D25" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" s="7" t="n">
+      <c r="E25" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G25" s="0" t="n">
@@ -2226,10 +2245,10 @@
         <v>600</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K25" s="1" t="n">
         <v>1</v>
@@ -2238,31 +2257,31 @@
         <v>2</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O25" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O25" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P25" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q25" s="9" t="s">
+      <c r="P25" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q25" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R25" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="T25" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="W25" s="0" t="n">
         <v>8149214985</v>
@@ -2273,21 +2292,21 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="7" t="n">
+      <c r="E26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G26" s="0" t="n">
@@ -2297,10 +2316,10 @@
         <v>600</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="K26" s="1" t="n">
         <v>1</v>
@@ -2309,28 +2328,28 @@
         <v>2</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O26" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O26" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P26" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q26" s="9" t="s">
-        <v>108</v>
+      <c r="P26" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q26" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="T26" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="U26" s="0" t="n">
         <v>123456765445434</v>
@@ -2339,7 +2358,7 @@
         <v>8149214985</v>
       </c>
       <c r="X26" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Y26" s="1" t="n">
         <v>791113</v>
@@ -2347,21 +2366,21 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D27" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="7" t="n">
+      <c r="E27" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G27" s="0" t="n">
@@ -2371,10 +2390,10 @@
         <v>600</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="K27" s="1" t="n">
         <v>1</v>
@@ -2383,31 +2402,31 @@
         <v>2</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O27" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O27" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P27" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q27" s="9" t="s">
+      <c r="P27" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q27" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="T27" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="V27" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="Y27" s="0" t="n">
         <v>411001</v>
@@ -2415,21 +2434,21 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D28" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="7" t="n">
+      <c r="E28" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G28" s="0" t="n">
@@ -2439,10 +2458,10 @@
         <v>600</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="K28" s="1" t="n">
         <v>1</v>
@@ -2451,25 +2470,25 @@
         <v>2</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O28" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O28" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P28" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q28" s="9" t="s">
+      <c r="P28" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q28" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R28" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="W28" s="0" t="n">
         <v>656765</v>
@@ -2477,21 +2496,21 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D29" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F29" s="7" t="n">
+      <c r="E29" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G29" s="0" t="n">
@@ -2501,10 +2520,10 @@
         <v>600</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K29" s="1" t="n">
         <v>1</v>
@@ -2513,44 +2532,44 @@
         <v>1</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O29" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O29" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P29" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q29" s="9" t="s">
+      <c r="P29" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q29" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R29" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D30" s="2" t="n">
         <v>123456</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="7" t="n">
+      <c r="E30" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="G30" s="0" t="n">
@@ -2560,10 +2579,10 @@
         <v>600</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="K30" s="1" t="n">
         <v>1</v>
@@ -2572,22 +2591,22 @@
         <v>1</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O30" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="O30" s="10" t="n">
         <v>45386</v>
       </c>
-      <c r="P30" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q30" s="9" t="s">
+      <c r="P30" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="Q30" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="R30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S30" s="3"/>
     </row>
@@ -2595,331 +2614,331 @@
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
       <c r="I31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
       <c r="S31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="8"/>
       <c r="I32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
       <c r="S32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
       <c r="I33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
       <c r="S33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
       <c r="I34" s="1"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
       <c r="S34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="8"/>
       <c r="I35" s="1"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
       <c r="S35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="8"/>
       <c r="I36" s="1"/>
       <c r="N36" s="1"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
       <c r="S36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="8"/>
       <c r="I37" s="1"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="9"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
       <c r="S37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="8"/>
       <c r="I38" s="1"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="9"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
       <c r="S38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="8"/>
       <c r="I39" s="1"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
       <c r="S39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="8"/>
       <c r="I40" s="1"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="9"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
       <c r="S40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="8"/>
       <c r="I41" s="1"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="9"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
       <c r="S41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
       <c r="I42" s="1"/>
-      <c r="O42" s="9"/>
-      <c r="P42" s="9"/>
-      <c r="Q42" s="9"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
       <c r="S42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
       <c r="I43" s="1"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
       <c r="S43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="8"/>
       <c r="I44" s="1"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
       <c r="S44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="8"/>
       <c r="I45" s="1"/>
-      <c r="O45" s="9"/>
-      <c r="P45" s="9"/>
-      <c r="Q45" s="9"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
       <c r="S45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="8"/>
       <c r="I46" s="1"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
       <c r="S46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="8"/>
       <c r="I47" s="1"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9"/>
-      <c r="Q47" s="9"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
       <c r="S47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="8"/>
       <c r="I48" s="1"/>
-      <c r="O48" s="9"/>
-      <c r="P48" s="9"/>
-      <c r="Q48" s="9"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
       <c r="S48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="8"/>
       <c r="I49" s="1"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="9"/>
-      <c r="Q49" s="9"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="10"/>
       <c r="S49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="8"/>
       <c r="I50" s="1"/>
-      <c r="O50" s="9"/>
-      <c r="P50" s="9"/>
-      <c r="Q50" s="9"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
       <c r="S50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="8"/>
       <c r="I51" s="1"/>
-      <c r="O51" s="9"/>
-      <c r="P51" s="9"/>
-      <c r="Q51" s="9"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
       <c r="S51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="8"/>
       <c r="I52" s="1"/>
-      <c r="O52" s="9"/>
-      <c r="P52" s="9"/>
-      <c r="Q52" s="9"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
       <c r="S52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="8"/>
       <c r="I53" s="1"/>
-      <c r="O53" s="9"/>
-      <c r="P53" s="9"/>
-      <c r="Q53" s="9"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="10"/>
       <c r="S53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="8"/>
       <c r="I54" s="1"/>
-      <c r="O54" s="9"/>
-      <c r="P54" s="9"/>
-      <c r="Q54" s="9"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="10"/>
+      <c r="Q54" s="10"/>
       <c r="S54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="8"/>
       <c r="I55" s="1"/>
-      <c r="O55" s="9"/>
-      <c r="P55" s="9"/>
-      <c r="Q55" s="9"/>
+      <c r="O55" s="10"/>
+      <c r="P55" s="10"/>
+      <c r="Q55" s="10"/>
       <c r="S55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="8"/>
       <c r="I56" s="1"/>
-      <c r="O56" s="9"/>
-      <c r="P56" s="9"/>
-      <c r="Q56" s="9"/>
+      <c r="O56" s="10"/>
+      <c r="P56" s="10"/>
+      <c r="Q56" s="10"/>
       <c r="S56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="8"/>
       <c r="I57" s="1"/>
-      <c r="O57" s="9"/>
-      <c r="P57" s="9"/>
-      <c r="Q57" s="9"/>
+      <c r="O57" s="10"/>
+      <c r="P57" s="10"/>
+      <c r="Q57" s="10"/>
       <c r="S57" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2929,9 +2948,9 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="I58" s="1"/>
-      <c r="O58" s="9"/>
-      <c r="P58" s="9"/>
-      <c r="Q58" s="9"/>
+      <c r="O58" s="10"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="10"/>
       <c r="S58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2941,9 +2960,9 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="I59" s="1"/>
-      <c r="O59" s="9"/>
-      <c r="P59" s="9"/>
-      <c r="Q59" s="9"/>
+      <c r="O59" s="10"/>
+      <c r="P59" s="10"/>
+      <c r="Q59" s="10"/>
       <c r="S59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2953,9 +2972,9 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="I60" s="1"/>
-      <c r="O60" s="9"/>
-      <c r="P60" s="9"/>
-      <c r="Q60" s="9"/>
+      <c r="O60" s="10"/>
+      <c r="P60" s="10"/>
+      <c r="Q60" s="10"/>
       <c r="S60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2965,9 +2984,9 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="I61" s="1"/>
-      <c r="O61" s="9"/>
-      <c r="P61" s="9"/>
-      <c r="Q61" s="9"/>
+      <c r="O61" s="10"/>
+      <c r="P61" s="10"/>
+      <c r="Q61" s="10"/>
       <c r="S61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2977,9 +2996,9 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="I62" s="1"/>
-      <c r="O62" s="9"/>
-      <c r="P62" s="9"/>
-      <c r="Q62" s="9"/>
+      <c r="O62" s="10"/>
+      <c r="P62" s="10"/>
+      <c r="Q62" s="10"/>
       <c r="S62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2989,9 +3008,9 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="I63" s="1"/>
-      <c r="O63" s="9"/>
-      <c r="P63" s="9"/>
-      <c r="Q63" s="9"/>
+      <c r="O63" s="10"/>
+      <c r="P63" s="10"/>
+      <c r="Q63" s="10"/>
       <c r="S63" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Search Invoice Keyword
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/customer_tagging_test_data.xlsx
+++ b/TestData/Web_POS/Billing/customer_tagging_test_data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr fullPrecision="1" calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,462 +19,471 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="124">
-  <si>
-    <t xml:space="preserve">TC_Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serial_key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username_admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password_admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username_pos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password_pos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">closing_balance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">opening_balance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">promo_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assortment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buy_items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">get_items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_invoice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">legal_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uin_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gst_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer_phone_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new_legal_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pincode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">salesperson_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new_city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">307260624P3E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zwshashank.agrawal@teampureplay.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">userone_p1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Index9QA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any___qty-Flat-Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118410781 : 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maharashtra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pune</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dummy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">307260624YP3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">usertwop10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any___qty-flat-Amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">307260624Wa9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any___qty-Flat-Fixed-Each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3070907243ZY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">userone_p9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any____qty-Flat-Fixed-All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118410781 : 2, 8906118412556 : 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saloni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any___qty-Buypool-Free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118410781 : 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any____qty-Getpool-Specificqty-Free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any____qty-Getpool-Anyqty-Free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Specificqty-Flat-percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Specificqty-Flat-rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Anyqty-Flat-percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any___qty-Buypool-Flat-percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118410781 : 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____qty-Buypool-Flat-Rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GST1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29GGGGG1314R9Z6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____qty-Buy Pool-fixed-each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118410781 : 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UIN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any Qty-Buy pool-Fixed-all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Existing GST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any Qty-get pool-spf-Rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GST2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any Qty-get pool-spf-Fixed-each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any Get pool-spf-Fixed-all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Specificity-Flat-fixed-all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete GST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delgst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Specificity-Flat-fixed-each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete UIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deluin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arunachalgst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12AAACB1534F1ZH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pasighat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UIN3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-fixed-each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-fixed-all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-spf-perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30AAAAP0267H1Z1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any qty-flat-rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arunachal Pradesh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Itanagar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any qty-flat-fixed-each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GST10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34565432345dfgfdfgfd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any qty-flat-fixed-all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSLB-flat-free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSLB-flat-perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118410781 : 4</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125" count="391">
+  <si>
+    <t>TC_Id</t>
+  </si>
+  <si>
+    <t>serial_key</t>
+  </si>
+  <si>
+    <t>username_admin</t>
+  </si>
+  <si>
+    <t>password_admin</t>
+  </si>
+  <si>
+    <t>username_pos</t>
+  </si>
+  <si>
+    <t>password_pos</t>
+  </si>
+  <si>
+    <t>closing_balance</t>
+  </si>
+  <si>
+    <t>opening_balance</t>
+  </si>
+  <si>
+    <t>store_name</t>
+  </si>
+  <si>
+    <t>promo_name</t>
+  </si>
+  <si>
+    <t>assortment</t>
+  </si>
+  <si>
+    <t>categories</t>
+  </si>
+  <si>
+    <t>buy_items</t>
+  </si>
+  <si>
+    <t>get_items</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>tax_invoice</t>
+  </si>
+  <si>
+    <t>legal_name</t>
+  </si>
+  <si>
+    <t>uin_number</t>
+  </si>
+  <si>
+    <t>gst_number</t>
+  </si>
+  <si>
+    <t>customer_phone_number</t>
+  </si>
+  <si>
+    <t>new_legal_name</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>salesperson_name</t>
+  </si>
+  <si>
+    <t>new_city</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>307260624P3E</t>
+  </si>
+  <si>
+    <t>zwshashank.agrawal@teampureplay.com</t>
+  </si>
+  <si>
+    <t>userone_p1 </t>
+  </si>
+  <si>
+    <t>Index9QA</t>
+  </si>
+  <si>
+    <t>QBSB-any___qty-Flat-Percentage</t>
+  </si>
+  <si>
+    <t>8906118410781 : 1</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>307260624YP3 </t>
+  </si>
+  <si>
+    <t>usertwop10 </t>
+  </si>
+  <si>
+    <t>QBSB-any___qty-flat-Amount</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>307260624Wa9</t>
+  </si>
+  <si>
+    <t>QBSB-any___qty-Flat-Fixed-Each</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>3070907243ZY</t>
+  </si>
+  <si>
+    <t>userone_p9</t>
+  </si>
+  <si>
+    <t>QBSB-any____qty-Flat-Fixed-All</t>
+  </si>
+  <si>
+    <t>8906118410781 : 2, 8906118412556 : 1</t>
+  </si>
+  <si>
+    <t>Saloni</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>QBSB-any___qty-Buypool-Free</t>
+  </si>
+  <si>
+    <t>8906118410781 : 2</t>
+  </si>
+  <si>
+    <t>TC_06</t>
+  </si>
+  <si>
+    <t>QBSB-any____qty-Getpool-Specificqty-Free</t>
+  </si>
+  <si>
+    <t>TC_07</t>
+  </si>
+  <si>
+    <t>QBSB-any____qty-Getpool-Anyqty-Free</t>
+  </si>
+  <si>
+    <t>TC_08</t>
+  </si>
+  <si>
+    <t>QBSB-Specificqty-Flat-percentage</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t>QBSB-Specificqty-Flat-rupees</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>QBSB-Anyqty-Flat-percentage</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>QBSB-Any___qty-Buypool-Flat-percentage</t>
+  </si>
+  <si>
+    <t>8906118410781 : 3</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>QBSB-Any____qty-Buypool-Flat-Rupees</t>
+  </si>
+  <si>
+    <t>GST1</t>
+  </si>
+  <si>
+    <t>29GGGGG1314R9Z6</t>
+  </si>
+  <si>
+    <t>TC_13</t>
+  </si>
+  <si>
+    <t>QBSB-Any____qty-Buy Pool-fixed-each</t>
+  </si>
+  <si>
+    <t>8906118410781 : 5</t>
+  </si>
+  <si>
+    <t>UIN1</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t>QBSB-Any Qty-Buy pool-Fixed-all</t>
+  </si>
+  <si>
+    <t>Existing GST</t>
+  </si>
+  <si>
+    <t>TC_15</t>
+  </si>
+  <si>
+    <t>QBSB-Any Qty-get pool-spf-Rupees</t>
+  </si>
+  <si>
+    <t>GST2</t>
+  </si>
+  <si>
+    <t>TC_16</t>
+  </si>
+  <si>
+    <t>QBSB-Any Qty-get pool-spf-Fixed-each</t>
+  </si>
+  <si>
+    <t>TC_17</t>
+  </si>
+  <si>
+    <t>QBSB-Any Get pool-spf-Fixed-all</t>
+  </si>
+  <si>
+    <t>TC_18</t>
+  </si>
+  <si>
+    <t>QBSB-Specificity-Flat-fixed-all</t>
+  </si>
+  <si>
+    <t>Delete GST</t>
+  </si>
+  <si>
+    <t>delgst</t>
+  </si>
+  <si>
+    <t>TC_19</t>
+  </si>
+  <si>
+    <t>QBSB-Specificity-Flat-fixed-each</t>
+  </si>
+  <si>
+    <t>Delete UIN</t>
+  </si>
+  <si>
+    <t>deluin</t>
+  </si>
+  <si>
+    <t>TC_20</t>
+  </si>
+  <si>
+    <t>QBSB-Any____Qty-get pool-any-perc</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>arunachalgst</t>
+  </si>
+  <si>
+    <t>12AAACB1534F1ZH </t>
+  </si>
+  <si>
+    <t>Pasighat</t>
+  </si>
+  <si>
+    <t>TC_21</t>
+  </si>
+  <si>
+    <t>QBSB-Any____Qty-get pool-any-rupees</t>
+  </si>
+  <si>
+    <t>UIN3</t>
+  </si>
+  <si>
+    <t>TC_22</t>
+  </si>
+  <si>
+    <t>QBSB-Any____Qty-get pool-any-fixed-each</t>
+  </si>
+  <si>
+    <t>TC_23</t>
+  </si>
+  <si>
+    <t>QBSB-Any____Qty-get pool-any-fixed-all</t>
+  </si>
+  <si>
+    <t>TC_24</t>
+  </si>
+  <si>
+    <t>QBSB-Any____Qty-get pool-spf-perc</t>
+  </si>
+  <si>
+    <t>30AAAAP0267H1Z1 </t>
+  </si>
+  <si>
+    <t>TC_25</t>
+  </si>
+  <si>
+    <t>QBSB-Any qty-flat-rupees</t>
+  </si>
+  <si>
+    <t>Arunachal Pradesh</t>
+  </si>
+  <si>
+    <t>Itanagar</t>
+  </si>
+  <si>
+    <t>TC_26</t>
+  </si>
+  <si>
+    <t>QBSB-Any qty-flat-fixed-each</t>
+  </si>
+  <si>
+    <t>GST10</t>
+  </si>
+  <si>
+    <t>34565432345dfgfdfgfd</t>
+  </si>
+  <si>
+    <t>TC_27</t>
+  </si>
+  <si>
+    <t>QBSB-Any qty-flat-fixed-all</t>
+  </si>
+  <si>
+    <t>TC_28</t>
+  </si>
+  <si>
+    <t>QBSLB-flat-free</t>
+  </si>
+  <si>
+    <t>TC_29</t>
+  </si>
+  <si>
+    <t>QBSLB-flat-perc</t>
+  </si>
+  <si>
+    <t>8906118410781 : 4</t>
+  </si>
+  <si>
+    <t>307260624Wa9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-409]M/D/YYYY"/>
+<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <charset val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF2B579A"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor indexed="64"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -483,16 +491,29 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E7E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+  <borders count="3">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color rgb="FF2B579A"/>
@@ -504,94 +525,66 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="37">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
@@ -600,6 +593,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="ConditionalFormatStyle" xfId="20"/>
     <cellStyle name="HeaderStyle" xfId="21"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -659,45 +653,51 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF2B579A"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AA63"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr/>
+  <dimension ref="A1:AMK63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+    <sheetView topLeftCell="L1" zoomScale="130" defaultGridColor="0" colorId="64" view="normal" tabSelected="1" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="39.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="28.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="1" width="29.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="23.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="28.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="12.63"/>
+    <col min="1" max="1" width="12.6796875" customWidth="1"/>
+    <col min="2" max="2" width="19.27734375" customWidth="1"/>
+    <col min="3" max="3" width="43.9296875" customWidth="1"/>
+    <col min="4" max="4" width="19.27734375" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.8203125" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="8" max="9" width="19.09765625" customWidth="1"/>
+    <col min="10" max="10" width="39.640625" style="1" customWidth="1"/>
+    <col min="11" max="12" width="31.95703125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="28.75" customWidth="1"/>
+    <col min="15" max="17" width="19.09765625" customWidth="1"/>
+    <col min="18" max="19" width="29.45703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="23.20703125" customWidth="1"/>
+    <col min="21" max="22" width="15" customWidth="1"/>
+    <col min="23" max="23" width="28.75" customWidth="1"/>
+    <col min="24" max="1025" width="12.6796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -715,13 +715,13 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -733,19 +733,19 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -779,8 +779,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:19" ht="33.75" customHeight="1">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -789,19 +789,19 @@
       <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="2">
         <v>123456</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G2" s="1" t="n">
+      <c r="F2" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G2" s="1">
         <v>1000</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1">
         <v>500</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -810,10 +810,10 @@
       <c r="J2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" s="1" t="n">
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
@@ -822,7 +822,7 @@
       <c r="N2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="10" t="n">
+      <c r="O2" s="10">
         <v>45386</v>
       </c>
       <c r="P2" s="10" t="s">
@@ -836,8 +836,8 @@
       </c>
       <c r="S2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:19" ht="19.5" customHeight="1">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -846,19 +846,19 @@
       <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="2">
         <v>123456</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G3" s="0" t="n">
+      <c r="F3" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G3">
         <v>1000</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3">
         <v>500</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -867,10 +867,10 @@
       <c r="J3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1" t="n">
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
         <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
@@ -879,7 +879,7 @@
       <c r="N3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="10" t="n">
+      <c r="O3" s="10">
         <v>45386</v>
       </c>
       <c r="P3" s="10" t="s">
@@ -893,29 +893,29 @@
       </c>
       <c r="S3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:19" ht="31.5" customHeight="1">
+      <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
+      <c r="B4" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="2">
         <v>123456</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G4" s="0" t="n">
+      <c r="F4" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G4">
         <v>1000</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4">
         <v>300</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -924,10 +924,10 @@
       <c r="J4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1" t="n">
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -936,7 +936,7 @@
       <c r="N4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="10" t="n">
+      <c r="O4" s="10">
         <v>45386</v>
       </c>
       <c r="P4" s="10" t="s">
@@ -950,8 +950,8 @@
       </c>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="34.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:26" ht="34.6" customHeight="1">
+      <c r="A5" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -960,19 +960,19 @@
       <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="2">
         <v>123456</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G5" s="0" t="n">
+      <c r="F5" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G5">
         <v>1000</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5">
         <v>400</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -981,10 +981,10 @@
       <c r="J5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1" t="n">
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
         <v>2</v>
       </c>
       <c r="M5" s="1" t="s">
@@ -993,7 +993,7 @@
       <c r="N5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="10" t="n">
+      <c r="O5" s="10">
         <v>45386</v>
       </c>
       <c r="P5" s="10" t="s">
@@ -1006,15 +1006,15 @@
         <v>37</v>
       </c>
       <c r="S5" s="3"/>
-      <c r="Y5" s="0" t="n">
+      <c r="Y5">
         <v>411001</v>
       </c>
-      <c r="Z5" s="0" t="s">
+      <c r="Z5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A6" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1023,19 +1023,19 @@
       <c r="C6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="2">
         <v>123456</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G6" s="0" t="n">
+      <c r="F6" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G6">
         <v>1000</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6">
         <v>800</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -1044,10 +1044,10 @@
       <c r="J6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1" t="n">
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
         <v>2</v>
       </c>
       <c r="M6" s="1" t="s">
@@ -1056,7 +1056,7 @@
       <c r="N6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="10" t="n">
+      <c r="O6" s="10">
         <v>45386</v>
       </c>
       <c r="P6" s="10" t="s">
@@ -1070,8 +1070,8 @@
       </c>
       <c r="S6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:19" ht="30" customHeight="1">
+      <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1080,19 +1080,19 @@
       <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="2">
         <v>123456</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G7" s="0" t="n">
+      <c r="F7" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G7">
         <v>1000</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7">
         <v>600</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -1101,10 +1101,10 @@
       <c r="J7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="K7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1" t="n">
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
         <v>2</v>
       </c>
       <c r="M7" s="1" t="s">
@@ -1113,7 +1113,7 @@
       <c r="N7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="10" t="n">
+      <c r="O7" s="10">
         <v>45386</v>
       </c>
       <c r="P7" s="10" t="s">
@@ -1127,8 +1127,8 @@
       </c>
       <c r="S7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:19" ht="31.5" customHeight="1">
+      <c r="A8" t="s">
         <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1137,19 +1137,19 @@
       <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="2">
         <v>123456</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G8" s="0" t="n">
+      <c r="F8" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G8">
         <v>1000</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8">
         <v>600</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -1158,10 +1158,10 @@
       <c r="J8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1" t="n">
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
         <v>2</v>
       </c>
       <c r="M8" s="1" t="s">
@@ -1170,7 +1170,7 @@
       <c r="N8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="10" t="n">
+      <c r="O8" s="10">
         <v>45386</v>
       </c>
       <c r="P8" s="10" t="s">
@@ -1184,8 +1184,8 @@
       </c>
       <c r="S8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:19" ht="32.25" customHeight="1">
+      <c r="A9" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1194,19 +1194,19 @@
       <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="2">
         <v>123456</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G9" s="0" t="n">
+      <c r="F9" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G9">
         <v>1000</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9">
         <v>600</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -1215,10 +1215,10 @@
       <c r="J9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" s="1" t="n">
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1">
         <v>2</v>
       </c>
       <c r="M9" s="1" t="s">
@@ -1227,7 +1227,7 @@
       <c r="N9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="10" t="n">
+      <c r="O9" s="10">
         <v>45386</v>
       </c>
       <c r="P9" s="10" t="s">
@@ -1241,8 +1241,8 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:23" ht="28.5" customHeight="1">
+      <c r="A10" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1251,19 +1251,19 @@
       <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="2">
         <v>123456</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G10" s="0" t="n">
+      <c r="F10" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G10">
         <v>1000</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10">
         <v>600</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -1272,10 +1272,10 @@
       <c r="J10" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="K10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L10" s="1" t="n">
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
         <v>2</v>
       </c>
       <c r="M10" s="1" t="s">
@@ -1284,7 +1284,7 @@
       <c r="N10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O10" s="10" t="n">
+      <c r="O10" s="10">
         <v>45386</v>
       </c>
       <c r="P10" s="10" t="s">
@@ -1297,12 +1297,12 @@
         <v>37</v>
       </c>
       <c r="S10" s="3"/>
-      <c r="W10" s="0" t="n">
+      <c r="W10">
         <v>9876543212</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:19" ht="14.3">
+      <c r="A11" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1311,19 +1311,19 @@
       <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="2">
         <v>123456</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G11" s="0" t="n">
+      <c r="F11" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G11">
         <v>1000</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11">
         <v>600</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -1332,10 +1332,10 @@
       <c r="J11" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="K11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" s="1" t="n">
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
         <v>2</v>
       </c>
       <c r="M11" s="1" t="s">
@@ -1344,7 +1344,7 @@
       <c r="N11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O11" s="10" t="n">
+      <c r="O11" s="10">
         <v>45386</v>
       </c>
       <c r="P11" s="10" t="s">
@@ -1358,8 +1358,8 @@
       </c>
       <c r="S11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:19" ht="14.3">
+      <c r="A12" t="s">
         <v>64</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1368,19 +1368,19 @@
       <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="2">
         <v>123456</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G12" s="0" t="n">
+      <c r="F12" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G12">
         <v>1000</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12">
         <v>600</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -1389,10 +1389,10 @@
       <c r="J12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="K12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1" t="n">
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
         <v>1</v>
       </c>
       <c r="M12" s="1" t="s">
@@ -1401,7 +1401,7 @@
       <c r="N12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O12" s="10" t="n">
+      <c r="O12" s="10">
         <v>45386</v>
       </c>
       <c r="P12" s="10" t="s">
@@ -1415,8 +1415,8 @@
       </c>
       <c r="S12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:25" ht="24.9">
+      <c r="A13" t="s">
         <v>67</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1425,19 +1425,19 @@
       <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="2">
         <v>123456</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G13" s="0" t="n">
+      <c r="F13" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G13">
         <v>1000</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13">
         <v>600</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -1446,10 +1446,10 @@
       <c r="J13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1" t="n">
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
         <v>1</v>
       </c>
       <c r="M13" s="1" t="s">
@@ -1458,7 +1458,7 @@
       <c r="N13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O13" s="10" t="n">
+      <c r="O13" s="10">
         <v>45386</v>
       </c>
       <c r="P13" s="10" t="s">
@@ -1471,18 +1471,18 @@
         <v>37</v>
       </c>
       <c r="S13" s="11"/>
-      <c r="T13" s="0" t="s">
+      <c r="T13" t="s">
         <v>69</v>
       </c>
       <c r="V13" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="Y13" s="0" t="n">
+      <c r="Y13">
         <v>411001</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:25" ht="24.9">
+      <c r="A14" t="s">
         <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1491,19 +1491,19 @@
       <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="2">
         <v>123456</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G14" s="0" t="n">
+      <c r="F14" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G14">
         <v>1000</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14">
         <v>600</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -1512,10 +1512,10 @@
       <c r="J14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L14" s="1" t="n">
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1">
         <v>1</v>
       </c>
       <c r="M14" s="1" t="s">
@@ -1524,7 +1524,7 @@
       <c r="N14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O14" s="10" t="n">
+      <c r="O14" s="10">
         <v>45386</v>
       </c>
       <c r="P14" s="10" t="s">
@@ -1537,18 +1537,18 @@
         <v>37</v>
       </c>
       <c r="S14" s="11"/>
-      <c r="T14" s="0" t="s">
+      <c r="T14" t="s">
         <v>74</v>
       </c>
       <c r="U14" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="Y14" s="0" t="n">
+      <c r="Y14">
         <v>411001</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:25" ht="13.8">
+      <c r="A15" t="s">
         <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1557,19 +1557,19 @@
       <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="2">
         <v>123456</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G15" s="0" t="n">
+      <c r="F15" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G15">
         <v>1000</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15">
         <v>600</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -1578,10 +1578,10 @@
       <c r="J15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L15" s="1" t="n">
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1">
         <v>1</v>
       </c>
       <c r="M15" s="1" t="s">
@@ -1590,7 +1590,7 @@
       <c r="N15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O15" s="10" t="n">
+      <c r="O15" s="10">
         <v>45386</v>
       </c>
       <c r="P15" s="10" t="s">
@@ -1605,18 +1605,18 @@
       <c r="S15" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="T15" s="0" t="s">
+      <c r="T15" t="s">
         <v>69</v>
       </c>
-      <c r="W15" s="0" t="n">
+      <c r="W15">
         <v>9876543212</v>
       </c>
-      <c r="Y15" s="0" t="n">
+      <c r="Y15">
         <v>411001</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:25" ht="13.8">
+      <c r="A16" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1625,19 +1625,19 @@
       <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="2">
         <v>123456</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G16" s="0" t="n">
+      <c r="F16" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G16">
         <v>1000</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16">
         <v>600</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -1646,10 +1646,10 @@
       <c r="J16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L16" s="1" t="n">
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1">
         <v>1</v>
       </c>
       <c r="M16" s="1" t="s">
@@ -1658,7 +1658,7 @@
       <c r="N16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O16" s="10" t="n">
+      <c r="O16" s="10">
         <v>45386</v>
       </c>
       <c r="P16" s="10" t="s">
@@ -1671,18 +1671,18 @@
         <v>37</v>
       </c>
       <c r="S16" s="3"/>
-      <c r="T16" s="0" t="s">
+      <c r="T16" t="s">
         <v>80</v>
       </c>
-      <c r="W16" s="0" t="n">
+      <c r="W16">
         <v>9876543212</v>
       </c>
-      <c r="Y16" s="0" t="n">
+      <c r="Y16">
         <v>411001</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:24" ht="13.8">
+      <c r="A17" t="s">
         <v>81</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1691,19 +1691,19 @@
       <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="2">
         <v>123456</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G17" s="0" t="n">
+      <c r="F17" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G17">
         <v>1000</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17">
         <v>600</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -1712,10 +1712,10 @@
       <c r="J17" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L17" s="1" t="n">
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
         <v>1</v>
       </c>
       <c r="M17" s="1" t="s">
@@ -1724,7 +1724,7 @@
       <c r="N17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O17" s="10" t="n">
+      <c r="O17" s="10">
         <v>45386</v>
       </c>
       <c r="P17" s="10" t="s">
@@ -1737,18 +1737,18 @@
         <v>37</v>
       </c>
       <c r="S17" s="3"/>
-      <c r="T17" s="0" t="s">
+      <c r="T17" t="s">
         <v>80</v>
       </c>
-      <c r="W17" s="0" t="n">
+      <c r="W17">
         <v>9876543212</v>
       </c>
-      <c r="X17" s="0" t="s">
+      <c r="X17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:24" ht="13.8">
+      <c r="A18" t="s">
         <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1757,19 +1757,19 @@
       <c r="C18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="2">
         <v>123456</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G18" s="0" t="n">
+      <c r="F18" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G18">
         <v>1000</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18">
         <v>600</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -1778,10 +1778,10 @@
       <c r="J18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L18" s="1" t="n">
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1">
         <v>3</v>
       </c>
       <c r="M18" s="1" t="s">
@@ -1790,7 +1790,7 @@
       <c r="N18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O18" s="10" t="n">
+      <c r="O18" s="10">
         <v>45386</v>
       </c>
       <c r="P18" s="10" t="s">
@@ -1803,18 +1803,18 @@
         <v>37</v>
       </c>
       <c r="S18" s="3"/>
-      <c r="T18" s="0" t="s">
+      <c r="T18" t="s">
         <v>69</v>
       </c>
-      <c r="W18" s="0" t="n">
+      <c r="W18">
         <v>9876543212</v>
       </c>
-      <c r="X18" s="0" t="s">
+      <c r="X18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:25" ht="24.9">
+      <c r="A19" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1823,19 +1823,19 @@
       <c r="C19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="D19" s="2">
         <v>123456</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G19" s="0" t="n">
+      <c r="F19" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G19">
         <v>1000</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19">
         <v>600</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -1844,10 +1844,10 @@
       <c r="J19" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L19" s="1" t="n">
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1">
         <v>1</v>
       </c>
       <c r="M19" s="1" t="s">
@@ -1856,7 +1856,7 @@
       <c r="N19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O19" s="10" t="n">
+      <c r="O19" s="10">
         <v>45386</v>
       </c>
       <c r="P19" s="10" t="s">
@@ -1871,7 +1871,7 @@
       <c r="S19" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="T19" s="0" t="s">
+      <c r="T19" t="s">
         <v>88</v>
       </c>
       <c r="U19" s="12" t="s">
@@ -1880,15 +1880,15 @@
       <c r="V19" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="W19" s="0" t="n">
+      <c r="W19">
         <v>8149214985</v>
       </c>
-      <c r="Y19" s="0" t="n">
+      <c r="Y19">
         <v>411001</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:25" ht="13.8">
+      <c r="A20" t="s">
         <v>89</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1897,19 +1897,19 @@
       <c r="C20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="2">
         <v>123456</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G20" s="0" t="n">
+      <c r="F20" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G20">
         <v>1000</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20">
         <v>600</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -1918,10 +1918,10 @@
       <c r="J20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K20" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L20" s="1" t="n">
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+      <c r="L20" s="1">
         <v>1</v>
       </c>
       <c r="M20" s="1" t="s">
@@ -1930,7 +1930,7 @@
       <c r="N20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O20" s="10" t="n">
+      <c r="O20" s="10">
         <v>45386</v>
       </c>
       <c r="P20" s="10" t="s">
@@ -1945,24 +1945,24 @@
       <c r="S20" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="T20" s="0" t="s">
+      <c r="T20" t="s">
         <v>92</v>
       </c>
-      <c r="U20" s="12" t="n">
+      <c r="U20" s="12">
         <v>123456789876543</v>
       </c>
-      <c r="V20" s="12" t="n">
+      <c r="V20" s="12">
         <v>123456789876543</v>
       </c>
-      <c r="W20" s="0" t="n">
+      <c r="W20">
         <v>8149214985</v>
       </c>
-      <c r="Y20" s="0" t="n">
+      <c r="Y20">
         <v>411001</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:27" ht="24.05">
+      <c r="A21" t="s">
         <v>93</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1971,19 +1971,19 @@
       <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="D21" s="2">
         <v>123456</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G21" s="0" t="n">
+      <c r="F21" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G21">
         <v>1000</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21">
         <v>600</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -1992,10 +1992,10 @@
       <c r="J21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K21" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L21" s="1" t="n">
+      <c r="K21" s="1">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1">
         <v>1</v>
       </c>
       <c r="M21" s="1" t="s">
@@ -2004,7 +2004,7 @@
       <c r="N21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O21" s="10" t="n">
+      <c r="O21" s="10">
         <v>45386</v>
       </c>
       <c r="P21" s="10" t="s">
@@ -2019,22 +2019,22 @@
       <c r="S21" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="T21" s="0" t="s">
+      <c r="T21" t="s">
         <v>96</v>
       </c>
       <c r="U21" s="1"/>
       <c r="V21" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="Y21" s="12" t="n">
+      <c r="Y21" s="12">
         <v>791102</v>
       </c>
-      <c r="AA21" s="0" t="s">
+      <c r="AA21" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:25" ht="13.8">
+      <c r="A22" t="s">
         <v>99</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2043,19 +2043,19 @@
       <c r="C22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D22" s="2">
         <v>123456</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G22" s="0" t="n">
+      <c r="F22" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G22">
         <v>1000</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22">
         <v>600</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -2064,19 +2064,19 @@
       <c r="J22" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K22" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L22" s="1" t="n">
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1">
         <v>3</v>
       </c>
-      <c r="M22" s="0" t="s">
+      <c r="M22" t="s">
         <v>53</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O22" s="10" t="n">
+      <c r="O22" s="10">
         <v>45386</v>
       </c>
       <c r="P22" s="10" t="s">
@@ -2091,18 +2091,18 @@
       <c r="S22" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="T22" s="0" t="s">
+      <c r="T22" t="s">
         <v>101</v>
       </c>
-      <c r="U22" s="0" t="n">
+      <c r="U22">
         <v>123456765445434</v>
       </c>
-      <c r="Y22" s="0" t="n">
+      <c r="Y22">
         <v>411001</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:25" ht="13.8">
+      <c r="A23" t="s">
         <v>102</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2111,19 +2111,19 @@
       <c r="C23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="D23" s="2">
         <v>123456</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G23" s="0" t="n">
+      <c r="F23" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G23">
         <v>1000</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23">
         <v>600</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -2132,19 +2132,19 @@
       <c r="J23" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K23" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L23" s="1" t="n">
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+      <c r="L23" s="1">
         <v>3</v>
       </c>
-      <c r="M23" s="0" t="s">
+      <c r="M23" t="s">
         <v>53</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O23" s="10" t="n">
+      <c r="O23" s="10">
         <v>45386</v>
       </c>
       <c r="P23" s="10" t="s">
@@ -2159,12 +2159,12 @@
       <c r="S23" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Y23" s="0" t="n">
+      <c r="Y23">
         <v>411001</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:25" ht="13.8">
+      <c r="A24" t="s">
         <v>104</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2173,19 +2173,19 @@
       <c r="C24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="2" t="n">
+      <c r="D24" s="2">
         <v>123456</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G24" s="0" t="n">
+      <c r="F24" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G24">
         <v>1000</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24">
         <v>600</v>
       </c>
       <c r="I24" s="1" t="s">
@@ -2194,16 +2194,16 @@
       <c r="J24" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L24" s="1" t="n">
+      <c r="L24" s="1">
         <v>2</v>
       </c>
-      <c r="M24" s="0" t="s">
+      <c r="M24" t="s">
         <v>53</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O24" s="10" t="n">
+      <c r="O24" s="10">
         <v>45386</v>
       </c>
       <c r="P24" s="10" t="s">
@@ -2218,12 +2218,12 @@
       <c r="S24" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Y24" s="0" t="n">
+      <c r="Y24">
         <v>411001</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:25" ht="24.9">
+      <c r="A25" t="s">
         <v>106</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2232,19 +2232,19 @@
       <c r="C25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="D25" s="2">
         <v>123456</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G25" s="0" t="n">
+      <c r="F25" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G25">
         <v>1000</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25">
         <v>600</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -2253,19 +2253,19 @@
       <c r="J25" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L25" s="1" t="n">
+      <c r="K25" s="1">
+        <v>1</v>
+      </c>
+      <c r="L25" s="1">
         <v>2</v>
       </c>
-      <c r="M25" s="0" t="s">
+      <c r="M25" t="s">
         <v>33</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O25" s="10" t="n">
+      <c r="O25" s="10">
         <v>45386</v>
       </c>
       <c r="P25" s="10" t="s">
@@ -2280,21 +2280,21 @@
       <c r="S25" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="T25" s="0" t="s">
+      <c r="T25" t="s">
         <v>88</v>
       </c>
       <c r="V25" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="W25" s="0" t="n">
+      <c r="W25">
         <v>8149214985</v>
       </c>
-      <c r="Y25" s="0" t="n">
+      <c r="Y25">
         <v>411001</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:25" ht="13.8">
+      <c r="A26" t="s">
         <v>109</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2303,19 +2303,19 @@
       <c r="C26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="D26" s="2">
         <v>123456</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F26" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G26" s="0" t="n">
+      <c r="F26" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G26">
         <v>1000</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26">
         <v>600</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -2324,19 +2324,19 @@
       <c r="J26" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="K26" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L26" s="1" t="n">
+      <c r="K26" s="1">
+        <v>1</v>
+      </c>
+      <c r="L26" s="1">
         <v>2</v>
       </c>
-      <c r="M26" s="0" t="s">
+      <c r="M26" t="s">
         <v>33</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O26" s="10" t="n">
+      <c r="O26" s="10">
         <v>45386</v>
       </c>
       <c r="P26" s="10" t="s">
@@ -2351,24 +2351,24 @@
       <c r="S26" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="T26" s="0" t="s">
+      <c r="T26" t="s">
         <v>92</v>
       </c>
-      <c r="U26" s="0" t="n">
+      <c r="U26">
         <v>123456765445434</v>
       </c>
-      <c r="W26" s="0" t="n">
+      <c r="W26">
         <v>8149214985</v>
       </c>
-      <c r="X26" s="0" t="s">
+      <c r="X26" t="s">
         <v>80</v>
       </c>
-      <c r="Y26" s="1" t="n">
+      <c r="Y26" s="1">
         <v>791113</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:25" ht="13.8">
+      <c r="A27" t="s">
         <v>113</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2377,19 +2377,19 @@
       <c r="C27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="2" t="n">
+      <c r="D27" s="2">
         <v>123456</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G27" s="0" t="n">
+      <c r="F27" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G27">
         <v>1000</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27">
         <v>600</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -2398,19 +2398,19 @@
       <c r="J27" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K27" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L27" s="1" t="n">
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+      <c r="L27" s="1">
         <v>2</v>
       </c>
-      <c r="M27" s="0" t="s">
+      <c r="M27" t="s">
         <v>33</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O27" s="10" t="n">
+      <c r="O27" s="10">
         <v>45386</v>
       </c>
       <c r="P27" s="10" t="s">
@@ -2425,18 +2425,18 @@
       <c r="S27" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="T27" s="0" t="s">
+      <c r="T27" t="s">
         <v>115</v>
       </c>
-      <c r="V27" s="0" t="s">
+      <c r="V27" t="s">
         <v>116</v>
       </c>
-      <c r="Y27" s="0" t="n">
+      <c r="Y27">
         <v>411001</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:23" ht="13.8">
+      <c r="A28" t="s">
         <v>117</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2445,19 +2445,19 @@
       <c r="C28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="2" t="n">
+      <c r="D28" s="2">
         <v>123456</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F28" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G28" s="0" t="n">
+      <c r="F28" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G28">
         <v>1000</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28">
         <v>600</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -2466,19 +2466,19 @@
       <c r="J28" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="K28" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L28" s="1" t="n">
+      <c r="K28" s="1">
+        <v>1</v>
+      </c>
+      <c r="L28" s="1">
         <v>2</v>
       </c>
-      <c r="M28" s="0" t="s">
+      <c r="M28" t="s">
         <v>33</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O28" s="10" t="n">
+      <c r="O28" s="10">
         <v>45386</v>
       </c>
       <c r="P28" s="10" t="s">
@@ -2493,12 +2493,12 @@
       <c r="S28" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="W28" s="0" t="n">
+      <c r="W28">
         <v>656765</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:19" ht="13.8">
+      <c r="A29" t="s">
         <v>119</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2507,19 +2507,19 @@
       <c r="C29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="2" t="n">
+      <c r="D29" s="2">
         <v>123456</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G29" s="0" t="n">
+      <c r="F29" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G29">
         <v>1000</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29">
         <v>600</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -2528,10 +2528,10 @@
       <c r="J29" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="K29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L29" s="1" t="n">
+      <c r="K29" s="1">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1">
         <v>1</v>
       </c>
       <c r="M29" s="1" t="s">
@@ -2540,7 +2540,7 @@
       <c r="N29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O29" s="10" t="n">
+      <c r="O29" s="10">
         <v>45386</v>
       </c>
       <c r="P29" s="10" t="s">
@@ -2556,8 +2556,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:19" ht="13.8">
+      <c r="A30" t="s">
         <v>121</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2566,19 +2566,19 @@
       <c r="C30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="2" t="n">
+      <c r="D30" s="2">
         <v>123456</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F30" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G30" s="0" t="n">
+      <c r="F30" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G30">
         <v>1000</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30">
         <v>600</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -2587,10 +2587,10 @@
       <c r="J30" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="K30" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L30" s="1" t="n">
+      <c r="K30" s="1">
+        <v>1</v>
+      </c>
+      <c r="L30" s="1">
         <v>1</v>
       </c>
       <c r="M30" s="1" t="s">
@@ -2599,7 +2599,7 @@
       <c r="N30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O30" s="10" t="n">
+      <c r="O30" s="10">
         <v>45386</v>
       </c>
       <c r="P30" s="10" t="s">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="S30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="2:19" ht="13.8">
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -2627,7 +2627,7 @@
       <c r="Q31" s="10"/>
       <c r="S31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="2:19" ht="13.8">
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -2641,7 +2641,7 @@
       <c r="Q32" s="10"/>
       <c r="S32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="2:19" ht="13.8">
       <c r="B33" s="1"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -2655,7 +2655,7 @@
       <c r="Q33" s="10"/>
       <c r="S33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="2:19" ht="13.8">
       <c r="B34" s="1"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -2667,7 +2667,7 @@
       <c r="Q34" s="10"/>
       <c r="S34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="2:19" ht="13.8">
       <c r="B35" s="1"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2679,7 +2679,7 @@
       <c r="Q35" s="10"/>
       <c r="S35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="2:19" ht="13.8">
       <c r="B36" s="1"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2692,7 +2692,7 @@
       <c r="Q36" s="10"/>
       <c r="S36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="2:19" ht="13.8">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2704,7 +2704,7 @@
       <c r="Q37" s="10"/>
       <c r="S37" s="3"/>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="2:19" ht="13.8">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -2716,7 +2716,7 @@
       <c r="Q38" s="10"/>
       <c r="S38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="2:19" ht="13.8">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2728,7 +2728,7 @@
       <c r="Q39" s="10"/>
       <c r="S39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="2:19" ht="13.8">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2740,7 +2740,7 @@
       <c r="Q40" s="10"/>
       <c r="S40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="2:19" ht="13.8">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2752,7 +2752,7 @@
       <c r="Q41" s="10"/>
       <c r="S41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="2:19" ht="13.8">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2764,7 +2764,7 @@
       <c r="Q42" s="10"/>
       <c r="S42" s="3"/>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="2:19" ht="13.8">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2776,7 +2776,7 @@
       <c r="Q43" s="10"/>
       <c r="S43" s="3"/>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="2:19" ht="13.8">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2788,7 +2788,7 @@
       <c r="Q44" s="10"/>
       <c r="S44" s="3"/>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="2:19" ht="13.8">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2800,7 +2800,7 @@
       <c r="Q45" s="10"/>
       <c r="S45" s="3"/>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="2:19" ht="13.8">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -2812,7 +2812,7 @@
       <c r="Q46" s="10"/>
       <c r="S46" s="3"/>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="2:19" ht="13.8">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -2824,7 +2824,7 @@
       <c r="Q47" s="10"/>
       <c r="S47" s="3"/>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="2:19" ht="13.8">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -2836,7 +2836,7 @@
       <c r="Q48" s="10"/>
       <c r="S48" s="3"/>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="2:19" ht="13.8">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2848,7 +2848,7 @@
       <c r="Q49" s="10"/>
       <c r="S49" s="3"/>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="2:19" ht="13.8">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -2860,7 +2860,7 @@
       <c r="Q50" s="10"/>
       <c r="S50" s="3"/>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="2:19" ht="13.8">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -2872,7 +2872,7 @@
       <c r="Q51" s="10"/>
       <c r="S51" s="3"/>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="2:19" ht="13.8">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2884,7 +2884,7 @@
       <c r="Q52" s="10"/>
       <c r="S52" s="3"/>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="2:19" ht="13.8">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2896,7 +2896,7 @@
       <c r="Q53" s="10"/>
       <c r="S53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="2:19" ht="13.8">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -2908,7 +2908,7 @@
       <c r="Q54" s="10"/>
       <c r="S54" s="3"/>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="2:19" ht="13.8">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -2920,7 +2920,7 @@
       <c r="Q55" s="10"/>
       <c r="S55" s="3"/>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="2:19" ht="13.8">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -2932,7 +2932,7 @@
       <c r="Q56" s="10"/>
       <c r="S56" s="3"/>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="2:19" ht="13.8">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -2944,7 +2944,7 @@
       <c r="Q57" s="10"/>
       <c r="S57" s="3"/>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="2:19" ht="13.8">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -2956,7 +2956,7 @@
       <c r="Q58" s="10"/>
       <c r="S58" s="3"/>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="2:19" ht="13.8">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2968,7 +2968,7 @@
       <c r="Q59" s="10"/>
       <c r="S59" s="3"/>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="2:19" ht="13.8">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2980,7 +2980,7 @@
       <c r="Q60" s="10"/>
       <c r="S60" s="3"/>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="2:19" ht="13.8">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -2992,7 +2992,7 @@
       <c r="Q61" s="10"/>
       <c r="S61" s="3"/>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="2:19" ht="13.8">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -3004,7 +3004,7 @@
       <c r="Q62" s="10"/>
       <c r="S62" s="3"/>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="2:19" ht="13.8">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -3017,12 +3017,9 @@
       <c r="S63" s="3"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter scaleWithDoc="1" alignWithMargins="1" differentFirst="0" differentOddEven="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved errors of "Add to Cart", "Product Catalogue", "Carry Bag", "Keyboard Shortcuts", "Mode Of Payment", " Sales person", "Share Invoice" and "Split Payment"
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/customer_tagging_test_data.xlsx
+++ b/TestData/Web_POS/Billing/customer_tagging_test_data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr fullPrecision="1" calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,462 +19,471 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="124">
-  <si>
-    <t xml:space="preserve">TC_Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serial_key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username_admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password_admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username_pos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password_pos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">closing_balance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">opening_balance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">promo_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assortment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buy_items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">get_items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_invoice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">legal_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uin_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gst_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer_phone_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new_legal_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pincode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">salesperson_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new_city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">307260624P3E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zwshashank.agrawal@teampureplay.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">userone_p1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Index9QA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any___qty-Flat-Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118410781 : 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maharashtra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pune</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dummy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">307260624YP3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">usertwop10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any___qty-flat-Amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">307260624Wa9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any___qty-Flat-Fixed-Each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3070907243ZY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">userone_p9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any____qty-Flat-Fixed-All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118410781 : 2, 8906118412556 : 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saloni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any___qty-Buypool-Free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118410781 : 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any____qty-Getpool-Specificqty-Free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-any____qty-Getpool-Anyqty-Free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Specificqty-Flat-percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Specificqty-Flat-rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Anyqty-Flat-percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any___qty-Buypool-Flat-percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118410781 : 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____qty-Buypool-Flat-Rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GST1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29GGGGG1314R9Z6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____qty-Buy Pool-fixed-each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118410781 : 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UIN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any Qty-Buy pool-Fixed-all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Existing GST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any Qty-get pool-spf-Rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GST2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any Qty-get pool-spf-Fixed-each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any Get pool-spf-Fixed-all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Specificity-Flat-fixed-all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete GST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delgst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Specificity-Flat-fixed-each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete UIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deluin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arunachalgst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12AAACB1534F1ZH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pasighat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UIN3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-fixed-each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-any-fixed-all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any____Qty-get pool-spf-perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30AAAAP0267H1Z1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any qty-flat-rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arunachal Pradesh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Itanagar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any qty-flat-fixed-each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GST10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34565432345dfgfdfgfd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any qty-flat-fixed-all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSLB-flat-free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSLB-flat-perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118410781 : 4</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125" count="391">
+  <si>
+    <t>TC_Id</t>
+  </si>
+  <si>
+    <t>serial_key</t>
+  </si>
+  <si>
+    <t>username_admin</t>
+  </si>
+  <si>
+    <t>password_admin</t>
+  </si>
+  <si>
+    <t>username_pos</t>
+  </si>
+  <si>
+    <t>password_pos</t>
+  </si>
+  <si>
+    <t>closing_balance</t>
+  </si>
+  <si>
+    <t>opening_balance</t>
+  </si>
+  <si>
+    <t>store_name</t>
+  </si>
+  <si>
+    <t>promo_name</t>
+  </si>
+  <si>
+    <t>assortment</t>
+  </si>
+  <si>
+    <t>categories</t>
+  </si>
+  <si>
+    <t>buy_items</t>
+  </si>
+  <si>
+    <t>get_items</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>tax_invoice</t>
+  </si>
+  <si>
+    <t>legal_name</t>
+  </si>
+  <si>
+    <t>uin_number</t>
+  </si>
+  <si>
+    <t>gst_number</t>
+  </si>
+  <si>
+    <t>customer_phone_number</t>
+  </si>
+  <si>
+    <t>new_legal_name</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>salesperson_name</t>
+  </si>
+  <si>
+    <t>new_city</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>307260624P3E</t>
+  </si>
+  <si>
+    <t>zwshashank.agrawal@teampureplay.com</t>
+  </si>
+  <si>
+    <t>userone_p1 </t>
+  </si>
+  <si>
+    <t>Index9QA</t>
+  </si>
+  <si>
+    <t>QBSB-any___qty-Flat-Percentage</t>
+  </si>
+  <si>
+    <t>8906118410781 : 1</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>307260624YP3 </t>
+  </si>
+  <si>
+    <t>usertwop10 </t>
+  </si>
+  <si>
+    <t>QBSB-any___qty-flat-Amount</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>307260624Wa9</t>
+  </si>
+  <si>
+    <t>QBSB-any___qty-Flat-Fixed-Each</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>3070907243ZY</t>
+  </si>
+  <si>
+    <t>userone_p9</t>
+  </si>
+  <si>
+    <t>QBSB-any____qty-Flat-Fixed-All</t>
+  </si>
+  <si>
+    <t>8906118410781 : 2, 8906118412556 : 1</t>
+  </si>
+  <si>
+    <t>Saloni</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>QBSB-any___qty-Buypool-Free</t>
+  </si>
+  <si>
+    <t>8906118410781 : 2</t>
+  </si>
+  <si>
+    <t>TC_06</t>
+  </si>
+  <si>
+    <t>QBSB-any____qty-Getpool-Specificqty-Free</t>
+  </si>
+  <si>
+    <t>TC_07</t>
+  </si>
+  <si>
+    <t>QBSB-any____qty-Getpool-Anyqty-Free</t>
+  </si>
+  <si>
+    <t>TC_08</t>
+  </si>
+  <si>
+    <t>QBSB-Specificqty-Flat-percentage</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t>QBSB-Specificqty-Flat-rupees</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>QBSB-Anyqty-Flat-percentage</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>QBSB-Any___qty-Buypool-Flat-percentage</t>
+  </si>
+  <si>
+    <t>8906118410781 : 3</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>QBSB-Any____qty-Buypool-Flat-Rupees</t>
+  </si>
+  <si>
+    <t>GST1</t>
+  </si>
+  <si>
+    <t>29GGGGG1314R9Z6</t>
+  </si>
+  <si>
+    <t>TC_13</t>
+  </si>
+  <si>
+    <t>QBSB-Any____qty-Buy Pool-fixed-each</t>
+  </si>
+  <si>
+    <t>8906118410781 : 5</t>
+  </si>
+  <si>
+    <t>UIN1</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t>QBSB-Any Qty-Buy pool-Fixed-all</t>
+  </si>
+  <si>
+    <t>Existing GST</t>
+  </si>
+  <si>
+    <t>TC_15</t>
+  </si>
+  <si>
+    <t>QBSB-Any Qty-get pool-spf-Rupees</t>
+  </si>
+  <si>
+    <t>GST2</t>
+  </si>
+  <si>
+    <t>TC_16</t>
+  </si>
+  <si>
+    <t>QBSB-Any Qty-get pool-spf-Fixed-each</t>
+  </si>
+  <si>
+    <t>TC_17</t>
+  </si>
+  <si>
+    <t>QBSB-Any Get pool-spf-Fixed-all</t>
+  </si>
+  <si>
+    <t>TC_18</t>
+  </si>
+  <si>
+    <t>QBSB-Specificity-Flat-fixed-all</t>
+  </si>
+  <si>
+    <t>Delete GST</t>
+  </si>
+  <si>
+    <t>delgst</t>
+  </si>
+  <si>
+    <t>TC_19</t>
+  </si>
+  <si>
+    <t>QBSB-Specificity-Flat-fixed-each</t>
+  </si>
+  <si>
+    <t>Delete UIN</t>
+  </si>
+  <si>
+    <t>deluin</t>
+  </si>
+  <si>
+    <t>TC_20</t>
+  </si>
+  <si>
+    <t>QBSB-Any____Qty-get pool-any-perc</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>arunachalgst</t>
+  </si>
+  <si>
+    <t>12AAACB1534F1ZH </t>
+  </si>
+  <si>
+    <t>Pasighat</t>
+  </si>
+  <si>
+    <t>TC_21</t>
+  </si>
+  <si>
+    <t>QBSB-Any____Qty-get pool-any-rupees</t>
+  </si>
+  <si>
+    <t>UIN3</t>
+  </si>
+  <si>
+    <t>TC_22</t>
+  </si>
+  <si>
+    <t>QBSB-Any____Qty-get pool-any-fixed-each</t>
+  </si>
+  <si>
+    <t>TC_23</t>
+  </si>
+  <si>
+    <t>QBSB-Any____Qty-get pool-any-fixed-all</t>
+  </si>
+  <si>
+    <t>TC_24</t>
+  </si>
+  <si>
+    <t>QBSB-Any____Qty-get pool-spf-perc</t>
+  </si>
+  <si>
+    <t>30AAAAP0267H1Z1 </t>
+  </si>
+  <si>
+    <t>TC_25</t>
+  </si>
+  <si>
+    <t>QBSB-Any qty-flat-rupees</t>
+  </si>
+  <si>
+    <t>Arunachal Pradesh</t>
+  </si>
+  <si>
+    <t>Itanagar</t>
+  </si>
+  <si>
+    <t>TC_26</t>
+  </si>
+  <si>
+    <t>QBSB-Any qty-flat-fixed-each</t>
+  </si>
+  <si>
+    <t>GST10</t>
+  </si>
+  <si>
+    <t>34565432345dfgfdfgfd</t>
+  </si>
+  <si>
+    <t>TC_27</t>
+  </si>
+  <si>
+    <t>QBSB-Any qty-flat-fixed-all</t>
+  </si>
+  <si>
+    <t>TC_28</t>
+  </si>
+  <si>
+    <t>QBSLB-flat-free</t>
+  </si>
+  <si>
+    <t>TC_29</t>
+  </si>
+  <si>
+    <t>QBSLB-flat-perc</t>
+  </si>
+  <si>
+    <t>8906118410781 : 4</t>
+  </si>
+  <si>
+    <t>307260624Wa9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-409]M/D/YYYY"/>
+<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <charset val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF2B579A"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor indexed="64"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -483,16 +491,29 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E7E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+  <borders count="3">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color rgb="FF2B579A"/>
@@ -504,94 +525,66 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="37">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
@@ -600,6 +593,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="ConditionalFormatStyle" xfId="20"/>
     <cellStyle name="HeaderStyle" xfId="21"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -659,45 +653,51 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF2B579A"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AA63"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr/>
+  <dimension ref="A1:AMK63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+    <sheetView topLeftCell="L1" zoomScale="130" defaultGridColor="0" colorId="64" view="normal" tabSelected="1" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="39.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="28.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="1" width="29.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="23.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="28.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="12.63"/>
+    <col min="1" max="1" width="12.6796875" customWidth="1"/>
+    <col min="2" max="2" width="19.27734375" customWidth="1"/>
+    <col min="3" max="3" width="43.9296875" customWidth="1"/>
+    <col min="4" max="4" width="19.27734375" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.8203125" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="8" max="9" width="19.09765625" customWidth="1"/>
+    <col min="10" max="10" width="39.640625" style="1" customWidth="1"/>
+    <col min="11" max="12" width="31.95703125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="28.75" customWidth="1"/>
+    <col min="15" max="17" width="19.09765625" customWidth="1"/>
+    <col min="18" max="19" width="29.45703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="23.20703125" customWidth="1"/>
+    <col min="21" max="22" width="15" customWidth="1"/>
+    <col min="23" max="23" width="28.75" customWidth="1"/>
+    <col min="24" max="1025" width="12.6796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -715,13 +715,13 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -733,19 +733,19 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -779,8 +779,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:19" ht="33.75" customHeight="1">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -789,19 +789,19 @@
       <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="2">
         <v>123456</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G2" s="1" t="n">
+      <c r="F2" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G2" s="1">
         <v>1000</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1">
         <v>500</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -810,10 +810,10 @@
       <c r="J2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" s="1" t="n">
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
@@ -822,7 +822,7 @@
       <c r="N2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="10" t="n">
+      <c r="O2" s="10">
         <v>45386</v>
       </c>
       <c r="P2" s="10" t="s">
@@ -836,8 +836,8 @@
       </c>
       <c r="S2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:19" ht="19.5" customHeight="1">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -846,19 +846,19 @@
       <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="2">
         <v>123456</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G3" s="0" t="n">
+      <c r="F3" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G3">
         <v>1000</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3">
         <v>500</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -867,10 +867,10 @@
       <c r="J3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1" t="n">
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
         <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
@@ -879,7 +879,7 @@
       <c r="N3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="10" t="n">
+      <c r="O3" s="10">
         <v>45386</v>
       </c>
       <c r="P3" s="10" t="s">
@@ -893,29 +893,29 @@
       </c>
       <c r="S3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:19" ht="31.5" customHeight="1">
+      <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
+      <c r="B4" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="2">
         <v>123456</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G4" s="0" t="n">
+      <c r="F4" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G4">
         <v>1000</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4">
         <v>300</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -924,10 +924,10 @@
       <c r="J4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1" t="n">
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -936,7 +936,7 @@
       <c r="N4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="10" t="n">
+      <c r="O4" s="10">
         <v>45386</v>
       </c>
       <c r="P4" s="10" t="s">
@@ -950,8 +950,8 @@
       </c>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="34.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:26" ht="34.6" customHeight="1">
+      <c r="A5" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -960,19 +960,19 @@
       <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="2">
         <v>123456</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G5" s="0" t="n">
+      <c r="F5" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G5">
         <v>1000</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5">
         <v>400</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -981,10 +981,10 @@
       <c r="J5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1" t="n">
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
         <v>2</v>
       </c>
       <c r="M5" s="1" t="s">
@@ -993,7 +993,7 @@
       <c r="N5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="10" t="n">
+      <c r="O5" s="10">
         <v>45386</v>
       </c>
       <c r="P5" s="10" t="s">
@@ -1006,15 +1006,15 @@
         <v>37</v>
       </c>
       <c r="S5" s="3"/>
-      <c r="Y5" s="0" t="n">
+      <c r="Y5">
         <v>411001</v>
       </c>
-      <c r="Z5" s="0" t="s">
+      <c r="Z5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A6" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1023,19 +1023,19 @@
       <c r="C6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="2">
         <v>123456</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G6" s="0" t="n">
+      <c r="F6" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G6">
         <v>1000</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6">
         <v>800</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -1044,10 +1044,10 @@
       <c r="J6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1" t="n">
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
         <v>2</v>
       </c>
       <c r="M6" s="1" t="s">
@@ -1056,7 +1056,7 @@
       <c r="N6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="10" t="n">
+      <c r="O6" s="10">
         <v>45386</v>
       </c>
       <c r="P6" s="10" t="s">
@@ -1070,8 +1070,8 @@
       </c>
       <c r="S6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:19" ht="30" customHeight="1">
+      <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1080,19 +1080,19 @@
       <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="2">
         <v>123456</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G7" s="0" t="n">
+      <c r="F7" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G7">
         <v>1000</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7">
         <v>600</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -1101,10 +1101,10 @@
       <c r="J7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="K7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1" t="n">
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
         <v>2</v>
       </c>
       <c r="M7" s="1" t="s">
@@ -1113,7 +1113,7 @@
       <c r="N7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="10" t="n">
+      <c r="O7" s="10">
         <v>45386</v>
       </c>
       <c r="P7" s="10" t="s">
@@ -1127,8 +1127,8 @@
       </c>
       <c r="S7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:19" ht="31.5" customHeight="1">
+      <c r="A8" t="s">
         <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1137,19 +1137,19 @@
       <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="2">
         <v>123456</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G8" s="0" t="n">
+      <c r="F8" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G8">
         <v>1000</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8">
         <v>600</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -1158,10 +1158,10 @@
       <c r="J8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1" t="n">
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
         <v>2</v>
       </c>
       <c r="M8" s="1" t="s">
@@ -1170,7 +1170,7 @@
       <c r="N8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="10" t="n">
+      <c r="O8" s="10">
         <v>45386</v>
       </c>
       <c r="P8" s="10" t="s">
@@ -1184,8 +1184,8 @@
       </c>
       <c r="S8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:19" ht="32.25" customHeight="1">
+      <c r="A9" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1194,19 +1194,19 @@
       <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="2">
         <v>123456</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G9" s="0" t="n">
+      <c r="F9" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G9">
         <v>1000</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9">
         <v>600</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -1215,10 +1215,10 @@
       <c r="J9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" s="1" t="n">
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1">
         <v>2</v>
       </c>
       <c r="M9" s="1" t="s">
@@ -1227,7 +1227,7 @@
       <c r="N9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="10" t="n">
+      <c r="O9" s="10">
         <v>45386</v>
       </c>
       <c r="P9" s="10" t="s">
@@ -1241,8 +1241,8 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:23" ht="28.5" customHeight="1">
+      <c r="A10" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1251,19 +1251,19 @@
       <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="2">
         <v>123456</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G10" s="0" t="n">
+      <c r="F10" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G10">
         <v>1000</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10">
         <v>600</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -1272,10 +1272,10 @@
       <c r="J10" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="K10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L10" s="1" t="n">
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
         <v>2</v>
       </c>
       <c r="M10" s="1" t="s">
@@ -1284,7 +1284,7 @@
       <c r="N10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O10" s="10" t="n">
+      <c r="O10" s="10">
         <v>45386</v>
       </c>
       <c r="P10" s="10" t="s">
@@ -1297,12 +1297,12 @@
         <v>37</v>
       </c>
       <c r="S10" s="3"/>
-      <c r="W10" s="0" t="n">
+      <c r="W10">
         <v>9876543212</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:19" ht="14.3">
+      <c r="A11" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1311,19 +1311,19 @@
       <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="2">
         <v>123456</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G11" s="0" t="n">
+      <c r="F11" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G11">
         <v>1000</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11">
         <v>600</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -1332,10 +1332,10 @@
       <c r="J11" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="K11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" s="1" t="n">
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
         <v>2</v>
       </c>
       <c r="M11" s="1" t="s">
@@ -1344,7 +1344,7 @@
       <c r="N11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O11" s="10" t="n">
+      <c r="O11" s="10">
         <v>45386</v>
       </c>
       <c r="P11" s="10" t="s">
@@ -1358,8 +1358,8 @@
       </c>
       <c r="S11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:19" ht="14.3">
+      <c r="A12" t="s">
         <v>64</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1368,19 +1368,19 @@
       <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="2">
         <v>123456</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G12" s="0" t="n">
+      <c r="F12" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G12">
         <v>1000</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12">
         <v>600</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -1389,10 +1389,10 @@
       <c r="J12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="K12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1" t="n">
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
         <v>1</v>
       </c>
       <c r="M12" s="1" t="s">
@@ -1401,7 +1401,7 @@
       <c r="N12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O12" s="10" t="n">
+      <c r="O12" s="10">
         <v>45386</v>
       </c>
       <c r="P12" s="10" t="s">
@@ -1415,8 +1415,8 @@
       </c>
       <c r="S12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:25" ht="24.9">
+      <c r="A13" t="s">
         <v>67</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1425,19 +1425,19 @@
       <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="2">
         <v>123456</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G13" s="0" t="n">
+      <c r="F13" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G13">
         <v>1000</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13">
         <v>600</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -1446,10 +1446,10 @@
       <c r="J13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1" t="n">
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
         <v>1</v>
       </c>
       <c r="M13" s="1" t="s">
@@ -1458,7 +1458,7 @@
       <c r="N13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O13" s="10" t="n">
+      <c r="O13" s="10">
         <v>45386</v>
       </c>
       <c r="P13" s="10" t="s">
@@ -1471,18 +1471,18 @@
         <v>37</v>
       </c>
       <c r="S13" s="11"/>
-      <c r="T13" s="0" t="s">
+      <c r="T13" t="s">
         <v>69</v>
       </c>
       <c r="V13" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="Y13" s="0" t="n">
+      <c r="Y13">
         <v>411001</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:25" ht="24.9">
+      <c r="A14" t="s">
         <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1491,19 +1491,19 @@
       <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="2">
         <v>123456</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G14" s="0" t="n">
+      <c r="F14" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G14">
         <v>1000</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14">
         <v>600</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -1512,10 +1512,10 @@
       <c r="J14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L14" s="1" t="n">
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1">
         <v>1</v>
       </c>
       <c r="M14" s="1" t="s">
@@ -1524,7 +1524,7 @@
       <c r="N14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O14" s="10" t="n">
+      <c r="O14" s="10">
         <v>45386</v>
       </c>
       <c r="P14" s="10" t="s">
@@ -1537,18 +1537,18 @@
         <v>37</v>
       </c>
       <c r="S14" s="11"/>
-      <c r="T14" s="0" t="s">
+      <c r="T14" t="s">
         <v>74</v>
       </c>
       <c r="U14" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="Y14" s="0" t="n">
+      <c r="Y14">
         <v>411001</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:25" ht="13.8">
+      <c r="A15" t="s">
         <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1557,19 +1557,19 @@
       <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="2">
         <v>123456</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G15" s="0" t="n">
+      <c r="F15" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G15">
         <v>1000</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15">
         <v>600</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -1578,10 +1578,10 @@
       <c r="J15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L15" s="1" t="n">
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1">
         <v>1</v>
       </c>
       <c r="M15" s="1" t="s">
@@ -1590,7 +1590,7 @@
       <c r="N15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O15" s="10" t="n">
+      <c r="O15" s="10">
         <v>45386</v>
       </c>
       <c r="P15" s="10" t="s">
@@ -1605,18 +1605,18 @@
       <c r="S15" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="T15" s="0" t="s">
+      <c r="T15" t="s">
         <v>69</v>
       </c>
-      <c r="W15" s="0" t="n">
+      <c r="W15">
         <v>9876543212</v>
       </c>
-      <c r="Y15" s="0" t="n">
+      <c r="Y15">
         <v>411001</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:25" ht="13.8">
+      <c r="A16" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1625,19 +1625,19 @@
       <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="2">
         <v>123456</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G16" s="0" t="n">
+      <c r="F16" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G16">
         <v>1000</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16">
         <v>600</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -1646,10 +1646,10 @@
       <c r="J16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L16" s="1" t="n">
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1">
         <v>1</v>
       </c>
       <c r="M16" s="1" t="s">
@@ -1658,7 +1658,7 @@
       <c r="N16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O16" s="10" t="n">
+      <c r="O16" s="10">
         <v>45386</v>
       </c>
       <c r="P16" s="10" t="s">
@@ -1671,18 +1671,18 @@
         <v>37</v>
       </c>
       <c r="S16" s="3"/>
-      <c r="T16" s="0" t="s">
+      <c r="T16" t="s">
         <v>80</v>
       </c>
-      <c r="W16" s="0" t="n">
+      <c r="W16">
         <v>9876543212</v>
       </c>
-      <c r="Y16" s="0" t="n">
+      <c r="Y16">
         <v>411001</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:24" ht="13.8">
+      <c r="A17" t="s">
         <v>81</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1691,19 +1691,19 @@
       <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="2">
         <v>123456</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G17" s="0" t="n">
+      <c r="F17" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G17">
         <v>1000</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17">
         <v>600</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -1712,10 +1712,10 @@
       <c r="J17" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L17" s="1" t="n">
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
         <v>1</v>
       </c>
       <c r="M17" s="1" t="s">
@@ -1724,7 +1724,7 @@
       <c r="N17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O17" s="10" t="n">
+      <c r="O17" s="10">
         <v>45386</v>
       </c>
       <c r="P17" s="10" t="s">
@@ -1737,18 +1737,18 @@
         <v>37</v>
       </c>
       <c r="S17" s="3"/>
-      <c r="T17" s="0" t="s">
+      <c r="T17" t="s">
         <v>80</v>
       </c>
-      <c r="W17" s="0" t="n">
+      <c r="W17">
         <v>9876543212</v>
       </c>
-      <c r="X17" s="0" t="s">
+      <c r="X17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:24" ht="13.8">
+      <c r="A18" t="s">
         <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1757,19 +1757,19 @@
       <c r="C18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="2">
         <v>123456</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G18" s="0" t="n">
+      <c r="F18" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G18">
         <v>1000</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18">
         <v>600</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -1778,10 +1778,10 @@
       <c r="J18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L18" s="1" t="n">
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1">
         <v>3</v>
       </c>
       <c r="M18" s="1" t="s">
@@ -1790,7 +1790,7 @@
       <c r="N18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O18" s="10" t="n">
+      <c r="O18" s="10">
         <v>45386</v>
       </c>
       <c r="P18" s="10" t="s">
@@ -1803,18 +1803,18 @@
         <v>37</v>
       </c>
       <c r="S18" s="3"/>
-      <c r="T18" s="0" t="s">
+      <c r="T18" t="s">
         <v>69</v>
       </c>
-      <c r="W18" s="0" t="n">
+      <c r="W18">
         <v>9876543212</v>
       </c>
-      <c r="X18" s="0" t="s">
+      <c r="X18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:25" ht="24.9">
+      <c r="A19" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1823,19 +1823,19 @@
       <c r="C19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="D19" s="2">
         <v>123456</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G19" s="0" t="n">
+      <c r="F19" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G19">
         <v>1000</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19">
         <v>600</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -1844,10 +1844,10 @@
       <c r="J19" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L19" s="1" t="n">
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1">
         <v>1</v>
       </c>
       <c r="M19" s="1" t="s">
@@ -1856,7 +1856,7 @@
       <c r="N19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O19" s="10" t="n">
+      <c r="O19" s="10">
         <v>45386</v>
       </c>
       <c r="P19" s="10" t="s">
@@ -1871,7 +1871,7 @@
       <c r="S19" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="T19" s="0" t="s">
+      <c r="T19" t="s">
         <v>88</v>
       </c>
       <c r="U19" s="12" t="s">
@@ -1880,15 +1880,15 @@
       <c r="V19" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="W19" s="0" t="n">
+      <c r="W19">
         <v>8149214985</v>
       </c>
-      <c r="Y19" s="0" t="n">
+      <c r="Y19">
         <v>411001</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:25" ht="13.8">
+      <c r="A20" t="s">
         <v>89</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1897,19 +1897,19 @@
       <c r="C20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="2">
         <v>123456</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G20" s="0" t="n">
+      <c r="F20" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G20">
         <v>1000</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20">
         <v>600</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -1918,10 +1918,10 @@
       <c r="J20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K20" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L20" s="1" t="n">
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+      <c r="L20" s="1">
         <v>1</v>
       </c>
       <c r="M20" s="1" t="s">
@@ -1930,7 +1930,7 @@
       <c r="N20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O20" s="10" t="n">
+      <c r="O20" s="10">
         <v>45386</v>
       </c>
       <c r="P20" s="10" t="s">
@@ -1945,24 +1945,24 @@
       <c r="S20" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="T20" s="0" t="s">
+      <c r="T20" t="s">
         <v>92</v>
       </c>
-      <c r="U20" s="12" t="n">
+      <c r="U20" s="12">
         <v>123456789876543</v>
       </c>
-      <c r="V20" s="12" t="n">
+      <c r="V20" s="12">
         <v>123456789876543</v>
       </c>
-      <c r="W20" s="0" t="n">
+      <c r="W20">
         <v>8149214985</v>
       </c>
-      <c r="Y20" s="0" t="n">
+      <c r="Y20">
         <v>411001</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:27" ht="24.05">
+      <c r="A21" t="s">
         <v>93</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1971,19 +1971,19 @@
       <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="D21" s="2">
         <v>123456</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G21" s="0" t="n">
+      <c r="F21" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G21">
         <v>1000</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21">
         <v>600</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -1992,10 +1992,10 @@
       <c r="J21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K21" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L21" s="1" t="n">
+      <c r="K21" s="1">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1">
         <v>1</v>
       </c>
       <c r="M21" s="1" t="s">
@@ -2004,7 +2004,7 @@
       <c r="N21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O21" s="10" t="n">
+      <c r="O21" s="10">
         <v>45386</v>
       </c>
       <c r="P21" s="10" t="s">
@@ -2019,22 +2019,22 @@
       <c r="S21" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="T21" s="0" t="s">
+      <c r="T21" t="s">
         <v>96</v>
       </c>
       <c r="U21" s="1"/>
       <c r="V21" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="Y21" s="12" t="n">
+      <c r="Y21" s="12">
         <v>791102</v>
       </c>
-      <c r="AA21" s="0" t="s">
+      <c r="AA21" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:25" ht="13.8">
+      <c r="A22" t="s">
         <v>99</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2043,19 +2043,19 @@
       <c r="C22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D22" s="2">
         <v>123456</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G22" s="0" t="n">
+      <c r="F22" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G22">
         <v>1000</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22">
         <v>600</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -2064,19 +2064,19 @@
       <c r="J22" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K22" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L22" s="1" t="n">
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1">
         <v>3</v>
       </c>
-      <c r="M22" s="0" t="s">
+      <c r="M22" t="s">
         <v>53</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O22" s="10" t="n">
+      <c r="O22" s="10">
         <v>45386</v>
       </c>
       <c r="P22" s="10" t="s">
@@ -2091,18 +2091,18 @@
       <c r="S22" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="T22" s="0" t="s">
+      <c r="T22" t="s">
         <v>101</v>
       </c>
-      <c r="U22" s="0" t="n">
+      <c r="U22">
         <v>123456765445434</v>
       </c>
-      <c r="Y22" s="0" t="n">
+      <c r="Y22">
         <v>411001</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:25" ht="13.8">
+      <c r="A23" t="s">
         <v>102</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2111,19 +2111,19 @@
       <c r="C23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="D23" s="2">
         <v>123456</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G23" s="0" t="n">
+      <c r="F23" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G23">
         <v>1000</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23">
         <v>600</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -2132,19 +2132,19 @@
       <c r="J23" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K23" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L23" s="1" t="n">
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+      <c r="L23" s="1">
         <v>3</v>
       </c>
-      <c r="M23" s="0" t="s">
+      <c r="M23" t="s">
         <v>53</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O23" s="10" t="n">
+      <c r="O23" s="10">
         <v>45386</v>
       </c>
       <c r="P23" s="10" t="s">
@@ -2159,12 +2159,12 @@
       <c r="S23" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Y23" s="0" t="n">
+      <c r="Y23">
         <v>411001</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:25" ht="13.8">
+      <c r="A24" t="s">
         <v>104</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2173,19 +2173,19 @@
       <c r="C24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="2" t="n">
+      <c r="D24" s="2">
         <v>123456</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G24" s="0" t="n">
+      <c r="F24" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G24">
         <v>1000</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24">
         <v>600</v>
       </c>
       <c r="I24" s="1" t="s">
@@ -2194,16 +2194,16 @@
       <c r="J24" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L24" s="1" t="n">
+      <c r="L24" s="1">
         <v>2</v>
       </c>
-      <c r="M24" s="0" t="s">
+      <c r="M24" t="s">
         <v>53</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O24" s="10" t="n">
+      <c r="O24" s="10">
         <v>45386</v>
       </c>
       <c r="P24" s="10" t="s">
@@ -2218,12 +2218,12 @@
       <c r="S24" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Y24" s="0" t="n">
+      <c r="Y24">
         <v>411001</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="24.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:25" ht="24.9">
+      <c r="A25" t="s">
         <v>106</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2232,19 +2232,19 @@
       <c r="C25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="D25" s="2">
         <v>123456</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G25" s="0" t="n">
+      <c r="F25" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G25">
         <v>1000</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25">
         <v>600</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -2253,19 +2253,19 @@
       <c r="J25" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L25" s="1" t="n">
+      <c r="K25" s="1">
+        <v>1</v>
+      </c>
+      <c r="L25" s="1">
         <v>2</v>
       </c>
-      <c r="M25" s="0" t="s">
+      <c r="M25" t="s">
         <v>33</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O25" s="10" t="n">
+      <c r="O25" s="10">
         <v>45386</v>
       </c>
       <c r="P25" s="10" t="s">
@@ -2280,21 +2280,21 @@
       <c r="S25" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="T25" s="0" t="s">
+      <c r="T25" t="s">
         <v>88</v>
       </c>
       <c r="V25" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="W25" s="0" t="n">
+      <c r="W25">
         <v>8149214985</v>
       </c>
-      <c r="Y25" s="0" t="n">
+      <c r="Y25">
         <v>411001</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:25" ht="13.8">
+      <c r="A26" t="s">
         <v>109</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2303,19 +2303,19 @@
       <c r="C26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="D26" s="2">
         <v>123456</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F26" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G26" s="0" t="n">
+      <c r="F26" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G26">
         <v>1000</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26">
         <v>600</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -2324,19 +2324,19 @@
       <c r="J26" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="K26" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L26" s="1" t="n">
+      <c r="K26" s="1">
+        <v>1</v>
+      </c>
+      <c r="L26" s="1">
         <v>2</v>
       </c>
-      <c r="M26" s="0" t="s">
+      <c r="M26" t="s">
         <v>33</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O26" s="10" t="n">
+      <c r="O26" s="10">
         <v>45386</v>
       </c>
       <c r="P26" s="10" t="s">
@@ -2351,24 +2351,24 @@
       <c r="S26" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="T26" s="0" t="s">
+      <c r="T26" t="s">
         <v>92</v>
       </c>
-      <c r="U26" s="0" t="n">
+      <c r="U26">
         <v>123456765445434</v>
       </c>
-      <c r="W26" s="0" t="n">
+      <c r="W26">
         <v>8149214985</v>
       </c>
-      <c r="X26" s="0" t="s">
+      <c r="X26" t="s">
         <v>80</v>
       </c>
-      <c r="Y26" s="1" t="n">
+      <c r="Y26" s="1">
         <v>791113</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:25" ht="13.8">
+      <c r="A27" t="s">
         <v>113</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2377,19 +2377,19 @@
       <c r="C27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="2" t="n">
+      <c r="D27" s="2">
         <v>123456</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G27" s="0" t="n">
+      <c r="F27" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G27">
         <v>1000</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27">
         <v>600</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -2398,19 +2398,19 @@
       <c r="J27" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K27" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L27" s="1" t="n">
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+      <c r="L27" s="1">
         <v>2</v>
       </c>
-      <c r="M27" s="0" t="s">
+      <c r="M27" t="s">
         <v>33</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O27" s="10" t="n">
+      <c r="O27" s="10">
         <v>45386</v>
       </c>
       <c r="P27" s="10" t="s">
@@ -2425,18 +2425,18 @@
       <c r="S27" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="T27" s="0" t="s">
+      <c r="T27" t="s">
         <v>115</v>
       </c>
-      <c r="V27" s="0" t="s">
+      <c r="V27" t="s">
         <v>116</v>
       </c>
-      <c r="Y27" s="0" t="n">
+      <c r="Y27">
         <v>411001</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:23" ht="13.8">
+      <c r="A28" t="s">
         <v>117</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2445,19 +2445,19 @@
       <c r="C28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="2" t="n">
+      <c r="D28" s="2">
         <v>123456</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F28" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G28" s="0" t="n">
+      <c r="F28" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G28">
         <v>1000</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28">
         <v>600</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -2466,19 +2466,19 @@
       <c r="J28" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="K28" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L28" s="1" t="n">
+      <c r="K28" s="1">
+        <v>1</v>
+      </c>
+      <c r="L28" s="1">
         <v>2</v>
       </c>
-      <c r="M28" s="0" t="s">
+      <c r="M28" t="s">
         <v>33</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O28" s="10" t="n">
+      <c r="O28" s="10">
         <v>45386</v>
       </c>
       <c r="P28" s="10" t="s">
@@ -2493,12 +2493,12 @@
       <c r="S28" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="W28" s="0" t="n">
+      <c r="W28">
         <v>656765</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:19" ht="13.8">
+      <c r="A29" t="s">
         <v>119</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2507,19 +2507,19 @@
       <c r="C29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="2" t="n">
+      <c r="D29" s="2">
         <v>123456</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G29" s="0" t="n">
+      <c r="F29" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G29">
         <v>1000</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29">
         <v>600</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -2528,10 +2528,10 @@
       <c r="J29" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="K29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L29" s="1" t="n">
+      <c r="K29" s="1">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1">
         <v>1</v>
       </c>
       <c r="M29" s="1" t="s">
@@ -2540,7 +2540,7 @@
       <c r="N29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O29" s="10" t="n">
+      <c r="O29" s="10">
         <v>45386</v>
       </c>
       <c r="P29" s="10" t="s">
@@ -2556,8 +2556,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:19" ht="13.8">
+      <c r="A30" t="s">
         <v>121</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2566,19 +2566,19 @@
       <c r="C30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="2" t="n">
+      <c r="D30" s="2">
         <v>123456</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F30" s="8" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G30" s="0" t="n">
+      <c r="F30" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G30">
         <v>1000</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30">
         <v>600</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -2587,10 +2587,10 @@
       <c r="J30" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="K30" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L30" s="1" t="n">
+      <c r="K30" s="1">
+        <v>1</v>
+      </c>
+      <c r="L30" s="1">
         <v>1</v>
       </c>
       <c r="M30" s="1" t="s">
@@ -2599,7 +2599,7 @@
       <c r="N30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O30" s="10" t="n">
+      <c r="O30" s="10">
         <v>45386</v>
       </c>
       <c r="P30" s="10" t="s">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="S30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="2:19" ht="13.8">
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -2627,7 +2627,7 @@
       <c r="Q31" s="10"/>
       <c r="S31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="2:19" ht="13.8">
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -2641,7 +2641,7 @@
       <c r="Q32" s="10"/>
       <c r="S32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="2:19" ht="13.8">
       <c r="B33" s="1"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -2655,7 +2655,7 @@
       <c r="Q33" s="10"/>
       <c r="S33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="2:19" ht="13.8">
       <c r="B34" s="1"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -2667,7 +2667,7 @@
       <c r="Q34" s="10"/>
       <c r="S34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="2:19" ht="13.8">
       <c r="B35" s="1"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2679,7 +2679,7 @@
       <c r="Q35" s="10"/>
       <c r="S35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="2:19" ht="13.8">
       <c r="B36" s="1"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2692,7 +2692,7 @@
       <c r="Q36" s="10"/>
       <c r="S36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="2:19" ht="13.8">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2704,7 +2704,7 @@
       <c r="Q37" s="10"/>
       <c r="S37" s="3"/>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="2:19" ht="13.8">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -2716,7 +2716,7 @@
       <c r="Q38" s="10"/>
       <c r="S38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="2:19" ht="13.8">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2728,7 +2728,7 @@
       <c r="Q39" s="10"/>
       <c r="S39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="2:19" ht="13.8">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2740,7 +2740,7 @@
       <c r="Q40" s="10"/>
       <c r="S40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="2:19" ht="13.8">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2752,7 +2752,7 @@
       <c r="Q41" s="10"/>
       <c r="S41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="2:19" ht="13.8">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2764,7 +2764,7 @@
       <c r="Q42" s="10"/>
       <c r="S42" s="3"/>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="2:19" ht="13.8">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2776,7 +2776,7 @@
       <c r="Q43" s="10"/>
       <c r="S43" s="3"/>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="2:19" ht="13.8">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2788,7 +2788,7 @@
       <c r="Q44" s="10"/>
       <c r="S44" s="3"/>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="2:19" ht="13.8">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2800,7 +2800,7 @@
       <c r="Q45" s="10"/>
       <c r="S45" s="3"/>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="2:19" ht="13.8">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -2812,7 +2812,7 @@
       <c r="Q46" s="10"/>
       <c r="S46" s="3"/>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="2:19" ht="13.8">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -2824,7 +2824,7 @@
       <c r="Q47" s="10"/>
       <c r="S47" s="3"/>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="2:19" ht="13.8">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -2836,7 +2836,7 @@
       <c r="Q48" s="10"/>
       <c r="S48" s="3"/>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="2:19" ht="13.8">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2848,7 +2848,7 @@
       <c r="Q49" s="10"/>
       <c r="S49" s="3"/>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="2:19" ht="13.8">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -2860,7 +2860,7 @@
       <c r="Q50" s="10"/>
       <c r="S50" s="3"/>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="2:19" ht="13.8">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -2872,7 +2872,7 @@
       <c r="Q51" s="10"/>
       <c r="S51" s="3"/>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="2:19" ht="13.8">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2884,7 +2884,7 @@
       <c r="Q52" s="10"/>
       <c r="S52" s="3"/>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="2:19" ht="13.8">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2896,7 +2896,7 @@
       <c r="Q53" s="10"/>
       <c r="S53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="2:19" ht="13.8">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -2908,7 +2908,7 @@
       <c r="Q54" s="10"/>
       <c r="S54" s="3"/>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="2:19" ht="13.8">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -2920,7 +2920,7 @@
       <c r="Q55" s="10"/>
       <c r="S55" s="3"/>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="2:19" ht="13.8">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -2932,7 +2932,7 @@
       <c r="Q56" s="10"/>
       <c r="S56" s="3"/>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="2:19" ht="13.8">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -2944,7 +2944,7 @@
       <c r="Q57" s="10"/>
       <c r="S57" s="3"/>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="2:19" ht="13.8">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -2956,7 +2956,7 @@
       <c r="Q58" s="10"/>
       <c r="S58" s="3"/>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="2:19" ht="13.8">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2968,7 +2968,7 @@
       <c r="Q59" s="10"/>
       <c r="S59" s="3"/>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="2:19" ht="13.8">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2980,7 +2980,7 @@
       <c r="Q60" s="10"/>
       <c r="S60" s="3"/>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="2:19" ht="13.8">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -2992,7 +2992,7 @@
       <c r="Q61" s="10"/>
       <c r="S61" s="3"/>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="2:19" ht="13.8">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -3004,7 +3004,7 @@
       <c r="Q62" s="10"/>
       <c r="S62" s="3"/>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="2:19" ht="13.8">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -3017,12 +3017,9 @@
       <c r="S63" s="3"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter scaleWithDoc="1" alignWithMargins="1" differentFirst="0" differentOddEven="0"/>
 </worksheet>
 </file>
</xml_diff>